<commit_message>
EB Replies part 2/2
</commit_message>
<xml_diff>
--- a/static/Users.xlsx
+++ b/static/Users.xlsx
@@ -454,9 +454,21 @@
           <t>OR001</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr"/>
-      <c r="C2" t="inlineStr"/>
-      <c r="D2" t="inlineStr"/>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Medha Iyer</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>medhaa642@gmail.com</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Ukraine</t>
+        </is>
+      </c>
       <c r="E2" t="inlineStr">
         <is>
           <t>557508</t>
@@ -469,9 +481,21 @@
           <t>OR002</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr"/>
-      <c r="C3" t="inlineStr"/>
-      <c r="D3" t="inlineStr"/>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Kritik Varshi</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>kritikvarshi@gmail.com</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>The Republic of Armenia</t>
+        </is>
+      </c>
       <c r="E3" t="inlineStr">
         <is>
           <t>318956</t>
@@ -484,9 +508,21 @@
           <t>OR003</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr"/>
-      <c r="C4" t="inlineStr"/>
-      <c r="D4" t="inlineStr"/>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Nikhil Vijay</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>nikhilpy123@gmail.com</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Hungary</t>
+        </is>
+      </c>
       <c r="E4" t="inlineStr">
         <is>
           <t>021322</t>
@@ -499,9 +535,21 @@
           <t>OR004</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr"/>
-      <c r="C5" t="inlineStr"/>
-      <c r="D5" t="inlineStr"/>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>V.Samhita</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>samhita191@gmail.com</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Republic of Bulgaria</t>
+        </is>
+      </c>
       <c r="E5" t="inlineStr">
         <is>
           <t>248785</t>
@@ -514,9 +562,21 @@
           <t>OR005</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr"/>
-      <c r="C6" t="inlineStr"/>
-      <c r="D6" t="inlineStr"/>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Kavya Hariharan</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>kaavyaa.hariharan@gmail.com</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>The Republic of Estonia</t>
+        </is>
+      </c>
       <c r="E6" t="inlineStr">
         <is>
           <t>808457</t>
@@ -544,9 +604,21 @@
           <t>OR007</t>
         </is>
       </c>
-      <c r="B8" t="inlineStr"/>
-      <c r="C8" t="inlineStr"/>
-      <c r="D8" t="inlineStr"/>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Varun S Mohan</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>vsm4710@gmail.com</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>The Argentine Republic</t>
+        </is>
+      </c>
       <c r="E8" t="inlineStr">
         <is>
           <t>213438</t>
@@ -559,9 +631,21 @@
           <t>OR008</t>
         </is>
       </c>
-      <c r="B9" t="inlineStr"/>
-      <c r="C9" t="inlineStr"/>
-      <c r="D9" t="inlineStr"/>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Pranav DS</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>pranavdevulapalli@yahoo.in</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>The Republic of Indonesia</t>
+        </is>
+      </c>
       <c r="E9" t="inlineStr">
         <is>
           <t>618750</t>
@@ -589,9 +673,21 @@
           <t>OR010</t>
         </is>
       </c>
-      <c r="B11" t="inlineStr"/>
-      <c r="C11" t="inlineStr"/>
-      <c r="D11" t="inlineStr"/>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Saroop Paul Carr</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>saroopcarr@gmail.com</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Republic of Korea</t>
+        </is>
+      </c>
       <c r="E11" t="inlineStr">
         <is>
           <t>183270</t>
@@ -604,9 +700,21 @@
           <t>OR011</t>
         </is>
       </c>
-      <c r="B12" t="inlineStr"/>
-      <c r="C12" t="inlineStr"/>
-      <c r="D12" t="inlineStr"/>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Ajan Sendhil</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>ajan.sendhil@gmail.com</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Republic of Turkey</t>
+        </is>
+      </c>
       <c r="E12" t="inlineStr">
         <is>
           <t>445914</t>
@@ -634,9 +742,21 @@
           <t>OR013</t>
         </is>
       </c>
-      <c r="B14" t="inlineStr"/>
-      <c r="C14" t="inlineStr"/>
-      <c r="D14" t="inlineStr"/>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Prahalad AV</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Prahaladvatsan@gmail.com</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Republic of Iraq</t>
+        </is>
+      </c>
       <c r="E14" t="inlineStr">
         <is>
           <t>758079</t>
@@ -649,9 +769,21 @@
           <t>OR014</t>
         </is>
       </c>
-      <c r="B15" t="inlineStr"/>
-      <c r="C15" t="inlineStr"/>
-      <c r="D15" t="inlineStr"/>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Bharath Vishal Ganesamoorthy</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>mgmsreviji@gmail.com</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>Islamic Republic of Pakistan</t>
+        </is>
+      </c>
       <c r="E15" t="inlineStr">
         <is>
           <t>948563</t>
@@ -664,9 +796,21 @@
           <t>OR015</t>
         </is>
       </c>
-      <c r="B16" t="inlineStr"/>
-      <c r="C16" t="inlineStr"/>
-      <c r="D16" t="inlineStr"/>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Charu Prabha</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>charu2010437@ssn.edu.in</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>The Republic of Croatia</t>
+        </is>
+      </c>
       <c r="E16" t="inlineStr">
         <is>
           <t>863454</t>
@@ -679,9 +823,21 @@
           <t>OR016</t>
         </is>
       </c>
-      <c r="B17" t="inlineStr"/>
-      <c r="C17" t="inlineStr"/>
-      <c r="D17" t="inlineStr"/>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Sriananthakamali S</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>sriananthakamali2011002@ssn.edu.in</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>The Kingdom of Denmark</t>
+        </is>
+      </c>
       <c r="E17" t="inlineStr">
         <is>
           <t>331114</t>
@@ -694,9 +850,21 @@
           <t>OR017</t>
         </is>
       </c>
-      <c r="B18" t="inlineStr"/>
-      <c r="C18" t="inlineStr"/>
-      <c r="D18" t="inlineStr"/>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Nithya Rajkumar</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>nithyaraj1506@gmail.com</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>The Republic of Belarus</t>
+        </is>
+      </c>
       <c r="E18" t="inlineStr">
         <is>
           <t>040916</t>
@@ -709,9 +877,21 @@
           <t>OR018</t>
         </is>
       </c>
-      <c r="B19" t="inlineStr"/>
-      <c r="C19" t="inlineStr"/>
-      <c r="D19" t="inlineStr"/>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Baghyashree P</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>pbaghyashree@gmail.com</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>The Hellenic Republic</t>
+        </is>
+      </c>
       <c r="E19" t="inlineStr">
         <is>
           <t>202580</t>
@@ -724,9 +904,21 @@
           <t>OR019</t>
         </is>
       </c>
-      <c r="B20" t="inlineStr"/>
-      <c r="C20" t="inlineStr"/>
-      <c r="D20" t="inlineStr"/>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Karun Anantharaman</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>karun19049@cse.ssn.edu.in</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>The Republic of Latvia</t>
+        </is>
+      </c>
       <c r="E20" t="inlineStr">
         <is>
           <t>077312</t>
@@ -739,9 +931,21 @@
           <t>OR020</t>
         </is>
       </c>
-      <c r="B21" t="inlineStr"/>
-      <c r="C21" t="inlineStr"/>
-      <c r="D21" t="inlineStr"/>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Sanjiv B N</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>sanjivbn777@gmail.com</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>The Republic of Poland</t>
+        </is>
+      </c>
       <c r="E21" t="inlineStr">
         <is>
           <t>423286</t>
@@ -769,9 +973,21 @@
           <t>OR022</t>
         </is>
       </c>
-      <c r="B23" t="inlineStr"/>
-      <c r="C23" t="inlineStr"/>
-      <c r="D23" t="inlineStr"/>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Lawrence Swaminathan</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>lawrence1seven@gmail.com</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>Kingdom of Spain</t>
+        </is>
+      </c>
       <c r="E23" t="inlineStr">
         <is>
           <t>443396</t>
@@ -784,9 +1000,21 @@
           <t>OR023</t>
         </is>
       </c>
-      <c r="B24" t="inlineStr"/>
-      <c r="C24" t="inlineStr"/>
-      <c r="D24" t="inlineStr"/>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Krisha Aarunee S</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>krishaaarunee@gmail.com</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>The Kingdom of Sweden</t>
+        </is>
+      </c>
       <c r="E24" t="inlineStr">
         <is>
           <t>251797</t>
@@ -829,9 +1057,21 @@
           <t>OR026</t>
         </is>
       </c>
-      <c r="B27" t="inlineStr"/>
-      <c r="C27" t="inlineStr"/>
-      <c r="D27" t="inlineStr"/>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Shravanthi</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>shravanthi2010346@ssn.edu.in</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>Republic of Cameroon</t>
+        </is>
+      </c>
       <c r="E27" t="inlineStr">
         <is>
           <t>306752</t>
@@ -844,9 +1084,21 @@
           <t>OR027</t>
         </is>
       </c>
-      <c r="B28" t="inlineStr"/>
-      <c r="C28" t="inlineStr"/>
-      <c r="D28" t="inlineStr"/>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Sushmitha srikanth</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>sushusri2002@gmail.com</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>Cote d' Ivorie</t>
+        </is>
+      </c>
       <c r="E28" t="inlineStr">
         <is>
           <t>824161</t>
@@ -874,9 +1126,21 @@
           <t>OR029</t>
         </is>
       </c>
-      <c r="B30" t="inlineStr"/>
-      <c r="C30" t="inlineStr"/>
-      <c r="D30" t="inlineStr"/>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Tanmay Pratti</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>tanmay2010168@ssn.edu.in</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>The Republic of Kazakhstan</t>
+        </is>
+      </c>
       <c r="E30" t="inlineStr">
         <is>
           <t>781595</t>
@@ -889,9 +1153,21 @@
           <t>OR030</t>
         </is>
       </c>
-      <c r="B31" t="inlineStr"/>
-      <c r="C31" t="inlineStr"/>
-      <c r="D31" t="inlineStr"/>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>Varun Deepak</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>varun2010089@ssn.edu.in</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>The Sultanate of Oman</t>
+        </is>
+      </c>
       <c r="E31" t="inlineStr">
         <is>
           <t>648509</t>
@@ -919,9 +1195,21 @@
           <t>OR032</t>
         </is>
       </c>
-      <c r="B33" t="inlineStr"/>
-      <c r="C33" t="inlineStr"/>
-      <c r="D33" t="inlineStr"/>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>Prabhakaran.P</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>prabha07lpm@gmail.com</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>The Republic of Austria</t>
+        </is>
+      </c>
       <c r="E33" t="inlineStr">
         <is>
           <t>879490</t>
@@ -934,9 +1222,21 @@
           <t>OR033</t>
         </is>
       </c>
-      <c r="B34" t="inlineStr"/>
-      <c r="C34" t="inlineStr"/>
-      <c r="D34" t="inlineStr"/>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>Aritra Karak</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>aritrakarak21@gmail.com</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>Russian Federation</t>
+        </is>
+      </c>
       <c r="E34" t="inlineStr">
         <is>
           <t>038366</t>
@@ -949,9 +1249,21 @@
           <t>OR034</t>
         </is>
       </c>
-      <c r="B35" t="inlineStr"/>
-      <c r="C35" t="inlineStr"/>
-      <c r="D35" t="inlineStr"/>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>Swastik Shukla</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>discoverswastik0411@gmail.com</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>The Republic of Azerbaijan</t>
+        </is>
+      </c>
       <c r="E35" t="inlineStr">
         <is>
           <t>768686</t>
@@ -994,9 +1306,21 @@
           <t>OR037</t>
         </is>
       </c>
-      <c r="B38" t="inlineStr"/>
-      <c r="C38" t="inlineStr"/>
-      <c r="D38" t="inlineStr"/>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>Hamsini Krishnan</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>hvrsini@gmail.com</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>The Kingdom of Saudi Arabia</t>
+        </is>
+      </c>
       <c r="E38" t="inlineStr">
         <is>
           <t>677738</t>
@@ -1009,9 +1333,21 @@
           <t>OR038</t>
         </is>
       </c>
-      <c r="B39" t="inlineStr"/>
-      <c r="C39" t="inlineStr"/>
-      <c r="D39" t="inlineStr"/>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>Sarthak Theurkar</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>sarthaktheurkar3@gmail.com</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>Kingdom of Belgium</t>
+        </is>
+      </c>
       <c r="E39" t="inlineStr">
         <is>
           <t>250614</t>
@@ -1024,9 +1360,21 @@
           <t>OR039</t>
         </is>
       </c>
-      <c r="B40" t="inlineStr"/>
-      <c r="C40" t="inlineStr"/>
-      <c r="D40" t="inlineStr"/>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>Ananya Ramakrishnan</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>ananyaramakrishnaa@gmail.com</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>The Republic of Lithuania</t>
+        </is>
+      </c>
       <c r="E40" t="inlineStr">
         <is>
           <t>534441</t>
@@ -1039,9 +1387,21 @@
           <t>OR040</t>
         </is>
       </c>
-      <c r="B41" t="inlineStr"/>
-      <c r="C41" t="inlineStr"/>
-      <c r="D41" t="inlineStr"/>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>Preetraj Raju Kurian</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>preetraj.prk2001@gmail.com</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>The Kingdom of Netherlands</t>
+        </is>
+      </c>
       <c r="E41" t="inlineStr">
         <is>
           <t>644817</t>
@@ -1084,9 +1444,21 @@
           <t>OR043</t>
         </is>
       </c>
-      <c r="B44" t="inlineStr"/>
-      <c r="C44" t="inlineStr"/>
-      <c r="D44" t="inlineStr"/>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>Anushree Appandairajan</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>anu.appandai@gmail.com</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>The Republic of Peru</t>
+        </is>
+      </c>
       <c r="E44" t="inlineStr">
         <is>
           <t>237657</t>
@@ -1189,9 +1561,21 @@
           <t>OR050</t>
         </is>
       </c>
-      <c r="B51" t="inlineStr"/>
-      <c r="C51" t="inlineStr"/>
-      <c r="D51" t="inlineStr"/>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>Anza Prem</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>anzaprem2002@gmail.com</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>The Republic of Ecuador</t>
+        </is>
+      </c>
       <c r="E51" t="inlineStr">
         <is>
           <t>700213</t>
@@ -1204,9 +1588,21 @@
           <t>OR051</t>
         </is>
       </c>
-      <c r="B52" t="inlineStr"/>
-      <c r="C52" t="inlineStr"/>
-      <c r="D52" t="inlineStr"/>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>Gurnehmat Dhindsa</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>gurnehmat.dhindsa@gmail.com</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>Swiss Confederation</t>
+        </is>
+      </c>
       <c r="E52" t="inlineStr">
         <is>
           <t>226153</t>
@@ -3454,9 +3850,21 @@
           <t>OR201</t>
         </is>
       </c>
-      <c r="B202" t="inlineStr"/>
-      <c r="C202" t="inlineStr"/>
-      <c r="D202" t="inlineStr"/>
+      <c r="B202" t="inlineStr">
+        <is>
+          <t>Varun R Swaminathan</t>
+        </is>
+      </c>
+      <c r="C202" t="inlineStr">
+        <is>
+          <t>varunrswaminathan@gmail.com</t>
+        </is>
+      </c>
+      <c r="D202" t="inlineStr">
+        <is>
+          <t>United States of America</t>
+        </is>
+      </c>
       <c r="E202" t="inlineStr">
         <is>
           <t>189993</t>
@@ -3469,9 +3877,21 @@
           <t>OR202</t>
         </is>
       </c>
-      <c r="B203" t="inlineStr"/>
-      <c r="C203" t="inlineStr"/>
-      <c r="D203" t="inlineStr"/>
+      <c r="B203" t="inlineStr">
+        <is>
+          <t>Advait Ramesh Kaluve</t>
+        </is>
+      </c>
+      <c r="C203" t="inlineStr">
+        <is>
+          <t>advaitkaluve@gmail.com</t>
+        </is>
+      </c>
+      <c r="D203" t="inlineStr">
+        <is>
+          <t>French Republic</t>
+        </is>
+      </c>
       <c r="E203" t="inlineStr">
         <is>
           <t>387186</t>
@@ -3484,9 +3904,21 @@
           <t>OR203</t>
         </is>
       </c>
-      <c r="B204" t="inlineStr"/>
-      <c r="C204" t="inlineStr"/>
-      <c r="D204" t="inlineStr"/>
+      <c r="B204" t="inlineStr">
+        <is>
+          <t>Tarun Aiyappa</t>
+        </is>
+      </c>
+      <c r="C204" t="inlineStr">
+        <is>
+          <t>tarunaiyappa26@gmail.com</t>
+        </is>
+      </c>
+      <c r="D204" t="inlineStr">
+        <is>
+          <t>United Kingdom of Great Britian and Northern Ireland</t>
+        </is>
+      </c>
       <c r="E204" t="inlineStr">
         <is>
           <t>930179</t>
@@ -3499,9 +3931,21 @@
           <t>OR204</t>
         </is>
       </c>
-      <c r="B205" t="inlineStr"/>
-      <c r="C205" t="inlineStr"/>
-      <c r="D205" t="inlineStr"/>
+      <c r="B205" t="inlineStr">
+        <is>
+          <t>Vedant Kumar Khetan</t>
+        </is>
+      </c>
+      <c r="C205" t="inlineStr">
+        <is>
+          <t>vedantkumarkhetan@gmail.com</t>
+        </is>
+      </c>
+      <c r="D205" t="inlineStr">
+        <is>
+          <t>The Republic of North Macedonia</t>
+        </is>
+      </c>
       <c r="E205" t="inlineStr">
         <is>
           <t>075859</t>
@@ -3514,9 +3958,21 @@
           <t>OR205</t>
         </is>
       </c>
-      <c r="B206" t="inlineStr"/>
-      <c r="C206" t="inlineStr"/>
-      <c r="D206" t="inlineStr"/>
+      <c r="B206" t="inlineStr">
+        <is>
+          <t>Bhargavi C</t>
+        </is>
+      </c>
+      <c r="C206" t="inlineStr">
+        <is>
+          <t>reenubhargavi9.11@gmail.com</t>
+        </is>
+      </c>
+      <c r="D206" t="inlineStr">
+        <is>
+          <t>The Commonwealth of Australia</t>
+        </is>
+      </c>
       <c r="E206" t="inlineStr">
         <is>
           <t>116215</t>
@@ -3529,9 +3985,21 @@
           <t>OR206</t>
         </is>
       </c>
-      <c r="B207" t="inlineStr"/>
-      <c r="C207" t="inlineStr"/>
-      <c r="D207" t="inlineStr"/>
+      <c r="B207" t="inlineStr">
+        <is>
+          <t>V.R.Nivedha Shalini</t>
+        </is>
+      </c>
+      <c r="C207" t="inlineStr">
+        <is>
+          <t>nivedha1937@bme.ssn.edu.in</t>
+        </is>
+      </c>
+      <c r="D207" t="inlineStr">
+        <is>
+          <t>The Federative Republic of Brazil</t>
+        </is>
+      </c>
       <c r="E207" t="inlineStr">
         <is>
           <t>211221</t>
@@ -3544,9 +4012,21 @@
           <t>OR207</t>
         </is>
       </c>
-      <c r="B208" t="inlineStr"/>
-      <c r="C208" t="inlineStr"/>
-      <c r="D208" t="inlineStr"/>
+      <c r="B208" t="inlineStr">
+        <is>
+          <t>R Swamenathan</t>
+        </is>
+      </c>
+      <c r="C208" t="inlineStr">
+        <is>
+          <t>swame2000@gmail.com</t>
+        </is>
+      </c>
+      <c r="D208" t="inlineStr">
+        <is>
+          <t>Canada</t>
+        </is>
+      </c>
       <c r="E208" t="inlineStr">
         <is>
           <t>880558</t>
@@ -3559,9 +4039,21 @@
           <t>OR208</t>
         </is>
       </c>
-      <c r="B209" t="inlineStr"/>
-      <c r="C209" t="inlineStr"/>
-      <c r="D209" t="inlineStr"/>
+      <c r="B209" t="inlineStr">
+        <is>
+          <t>Padma Malini R</t>
+        </is>
+      </c>
+      <c r="C209" t="inlineStr">
+        <is>
+          <t>padmamalini@live.in</t>
+        </is>
+      </c>
+      <c r="D209" t="inlineStr">
+        <is>
+          <t>The Republic of India</t>
+        </is>
+      </c>
       <c r="E209" t="inlineStr">
         <is>
           <t>596476</t>
@@ -3574,9 +4066,21 @@
           <t>OR209</t>
         </is>
       </c>
-      <c r="B210" t="inlineStr"/>
-      <c r="C210" t="inlineStr"/>
-      <c r="D210" t="inlineStr"/>
+      <c r="B210" t="inlineStr">
+        <is>
+          <t>Advaith Ganesh</t>
+        </is>
+      </c>
+      <c r="C210" t="inlineStr">
+        <is>
+          <t>advaith_g.sias19@krea.ac.in</t>
+        </is>
+      </c>
+      <c r="D210" t="inlineStr">
+        <is>
+          <t>The Republic of Italy</t>
+        </is>
+      </c>
       <c r="E210" t="inlineStr">
         <is>
           <t>683148</t>
@@ -3589,9 +4093,21 @@
           <t>OR210</t>
         </is>
       </c>
-      <c r="B211" t="inlineStr"/>
-      <c r="C211" t="inlineStr"/>
-      <c r="D211" t="inlineStr"/>
+      <c r="B211" t="inlineStr">
+        <is>
+          <t>Shinjini Chakraborty</t>
+        </is>
+      </c>
+      <c r="C211" t="inlineStr">
+        <is>
+          <t>shinjini.chakraborty2019@vitstudent.ac.in</t>
+        </is>
+      </c>
+      <c r="D211" t="inlineStr">
+        <is>
+          <t>The United Mexican States</t>
+        </is>
+      </c>
       <c r="E211" t="inlineStr">
         <is>
           <t>195421</t>
@@ -3604,9 +4120,21 @@
           <t>OR211</t>
         </is>
       </c>
-      <c r="B212" t="inlineStr"/>
-      <c r="C212" t="inlineStr"/>
-      <c r="D212" t="inlineStr"/>
+      <c r="B212" t="inlineStr">
+        <is>
+          <t>Raghav Ahuja</t>
+        </is>
+      </c>
+      <c r="C212" t="inlineStr">
+        <is>
+          <t>raghavahuja797@gmail.com</t>
+        </is>
+      </c>
+      <c r="D212" t="inlineStr">
+        <is>
+          <t>The Portuguese Republic</t>
+        </is>
+      </c>
       <c r="E212" t="inlineStr">
         <is>
           <t>186634</t>
@@ -3619,9 +4147,21 @@
           <t>OR212</t>
         </is>
       </c>
-      <c r="B213" t="inlineStr"/>
-      <c r="C213" t="inlineStr"/>
-      <c r="D213" t="inlineStr"/>
+      <c r="B213" t="inlineStr">
+        <is>
+          <t>Aditya Choudhary</t>
+        </is>
+      </c>
+      <c r="C213" t="inlineStr">
+        <is>
+          <t>crazyaditya11@gmail.com</t>
+        </is>
+      </c>
+      <c r="D213" t="inlineStr">
+        <is>
+          <t>Georgia</t>
+        </is>
+      </c>
       <c r="E213" t="inlineStr">
         <is>
           <t>617846</t>
@@ -10909,9 +11449,21 @@
           <t>OR698</t>
         </is>
       </c>
-      <c r="B699" t="inlineStr"/>
-      <c r="C699" t="inlineStr"/>
-      <c r="D699" t="inlineStr"/>
+      <c r="B699" t="inlineStr">
+        <is>
+          <t>Lawrence Swaminathan</t>
+        </is>
+      </c>
+      <c r="C699" t="inlineStr">
+        <is>
+          <t>veeravicky277@gmail.com</t>
+        </is>
+      </c>
+      <c r="D699" t="inlineStr">
+        <is>
+          <t>People's Republic of China</t>
+        </is>
+      </c>
       <c r="E699" t="inlineStr">
         <is>
           <t>559988</t>
@@ -10924,9 +11476,21 @@
           <t>OR699</t>
         </is>
       </c>
-      <c r="B700" t="inlineStr"/>
-      <c r="C700" t="inlineStr"/>
-      <c r="D700" t="inlineStr"/>
+      <c r="B700" t="inlineStr">
+        <is>
+          <t>Tanmay Pratti</t>
+        </is>
+      </c>
+      <c r="C700" t="inlineStr">
+        <is>
+          <t>harrineikumar@gmail.com</t>
+        </is>
+      </c>
+      <c r="D700" t="inlineStr">
+        <is>
+          <t>Russian Federation</t>
+        </is>
+      </c>
       <c r="E700" t="inlineStr">
         <is>
           <t>986606</t>
@@ -10954,9 +11518,21 @@
           <t>OR701</t>
         </is>
       </c>
-      <c r="B702" t="inlineStr"/>
-      <c r="C702" t="inlineStr"/>
-      <c r="D702" t="inlineStr"/>
+      <c r="B702" t="inlineStr">
+        <is>
+          <t>Sabariish Venkat</t>
+        </is>
+      </c>
+      <c r="C702" t="inlineStr">
+        <is>
+          <t>sabariishvenkat@gmail.com</t>
+        </is>
+      </c>
+      <c r="D702" t="inlineStr">
+        <is>
+          <t>International Press 1</t>
+        </is>
+      </c>
       <c r="E702" t="inlineStr">
         <is>
           <t>325614</t>
@@ -10984,9 +11560,21 @@
           <t>OR703</t>
         </is>
       </c>
-      <c r="B704" t="inlineStr"/>
-      <c r="C704" t="inlineStr"/>
-      <c r="D704" t="inlineStr"/>
+      <c r="B704" t="inlineStr">
+        <is>
+          <t>Suraksha Vinod</t>
+        </is>
+      </c>
+      <c r="C704" t="inlineStr">
+        <is>
+          <t>suraksha.vinod@gmail.com</t>
+        </is>
+      </c>
+      <c r="D704" t="inlineStr">
+        <is>
+          <t>International Press 2</t>
+        </is>
+      </c>
       <c r="E704" t="inlineStr">
         <is>
           <t>895618</t>
@@ -12439,9 +13027,21 @@
           <t>SC001</t>
         </is>
       </c>
-      <c r="B801" t="inlineStr"/>
-      <c r="C801" t="inlineStr"/>
-      <c r="D801" t="inlineStr"/>
+      <c r="B801" t="inlineStr">
+        <is>
+          <t>Adithiyha SK</t>
+        </is>
+      </c>
+      <c r="C801" t="inlineStr">
+        <is>
+          <t>skadithiyha2001@gmail.com</t>
+        </is>
+      </c>
+      <c r="D801" t="inlineStr">
+        <is>
+          <t>United Kingdom of Great Britain and Northern Ireland</t>
+        </is>
+      </c>
       <c r="E801" t="inlineStr">
         <is>
           <t>320071</t>
@@ -12484,9 +13084,21 @@
           <t>SC004</t>
         </is>
       </c>
-      <c r="B804" t="inlineStr"/>
-      <c r="C804" t="inlineStr"/>
-      <c r="D804" t="inlineStr"/>
+      <c r="B804" t="inlineStr">
+        <is>
+          <t>Dharun Aditya Senthilkumar</t>
+        </is>
+      </c>
+      <c r="C804" t="inlineStr">
+        <is>
+          <t>dharun2508@gmail.com</t>
+        </is>
+      </c>
+      <c r="D804" t="inlineStr">
+        <is>
+          <t>Ireland</t>
+        </is>
+      </c>
       <c r="E804" t="inlineStr">
         <is>
           <t>857227</t>
@@ -12499,9 +13111,21 @@
           <t>SC005</t>
         </is>
       </c>
-      <c r="B805" t="inlineStr"/>
-      <c r="C805" t="inlineStr"/>
-      <c r="D805" t="inlineStr"/>
+      <c r="B805" t="inlineStr">
+        <is>
+          <t>Adyant srinivasan</t>
+        </is>
+      </c>
+      <c r="C805" t="inlineStr">
+        <is>
+          <t>ad.srvn@gmail.com</t>
+        </is>
+      </c>
+      <c r="D805" t="inlineStr">
+        <is>
+          <t>Norway</t>
+        </is>
+      </c>
       <c r="E805" t="inlineStr">
         <is>
           <t>647795</t>
@@ -12514,9 +13138,21 @@
           <t>SC006</t>
         </is>
       </c>
-      <c r="B806" t="inlineStr"/>
-      <c r="C806" t="inlineStr"/>
-      <c r="D806" t="inlineStr"/>
+      <c r="B806" t="inlineStr">
+        <is>
+          <t>Gokul S</t>
+        </is>
+      </c>
+      <c r="C806" t="inlineStr">
+        <is>
+          <t>gokul.sundararaghavan132@gmail.com</t>
+        </is>
+      </c>
+      <c r="D806" t="inlineStr">
+        <is>
+          <t>Azerbaijan(O)</t>
+        </is>
+      </c>
       <c r="E806" t="inlineStr">
         <is>
           <t>342340</t>
@@ -12529,9 +13165,21 @@
           <t>SC007</t>
         </is>
       </c>
-      <c r="B807" t="inlineStr"/>
-      <c r="C807" t="inlineStr"/>
-      <c r="D807" t="inlineStr"/>
+      <c r="B807" t="inlineStr">
+        <is>
+          <t>Ashwin R</t>
+        </is>
+      </c>
+      <c r="C807" t="inlineStr">
+        <is>
+          <t>ashwin.achchu@gmail.com</t>
+        </is>
+      </c>
+      <c r="D807" t="inlineStr">
+        <is>
+          <t>Viet Nam</t>
+        </is>
+      </c>
       <c r="E807" t="inlineStr">
         <is>
           <t>331158</t>
@@ -12544,9 +13192,21 @@
           <t>SC008</t>
         </is>
       </c>
-      <c r="B808" t="inlineStr"/>
-      <c r="C808" t="inlineStr"/>
-      <c r="D808" t="inlineStr"/>
+      <c r="B808" t="inlineStr">
+        <is>
+          <t>Pranav Kumar</t>
+        </is>
+      </c>
+      <c r="C808" t="inlineStr">
+        <is>
+          <t>pran4vkumar@gmail.com</t>
+        </is>
+      </c>
+      <c r="D808" t="inlineStr">
+        <is>
+          <t>Tunisia</t>
+        </is>
+      </c>
       <c r="E808" t="inlineStr">
         <is>
           <t>485120</t>
@@ -12574,9 +13234,21 @@
           <t>SC010</t>
         </is>
       </c>
-      <c r="B810" t="inlineStr"/>
-      <c r="C810" t="inlineStr"/>
-      <c r="D810" t="inlineStr"/>
+      <c r="B810" t="inlineStr">
+        <is>
+          <t>Mrudhula Vijayakumar</t>
+        </is>
+      </c>
+      <c r="C810" t="inlineStr">
+        <is>
+          <t>vgnvjmp@gmail.com</t>
+        </is>
+      </c>
+      <c r="D810" t="inlineStr">
+        <is>
+          <t>Greece (O)</t>
+        </is>
+      </c>
       <c r="E810" t="inlineStr">
         <is>
           <t>261334</t>
@@ -12604,9 +13276,21 @@
           <t>SC012</t>
         </is>
       </c>
-      <c r="B812" t="inlineStr"/>
-      <c r="C812" t="inlineStr"/>
-      <c r="D812" t="inlineStr"/>
+      <c r="B812" t="inlineStr">
+        <is>
+          <t>Hrishikesh Jagannathan</t>
+        </is>
+      </c>
+      <c r="C812" t="inlineStr">
+        <is>
+          <t>nshrishekesh@gmail.com</t>
+        </is>
+      </c>
+      <c r="D812" t="inlineStr">
+        <is>
+          <t>Iran (O)</t>
+        </is>
+      </c>
       <c r="E812" t="inlineStr">
         <is>
           <t>437196</t>
@@ -12619,9 +13303,21 @@
           <t>SC013</t>
         </is>
       </c>
-      <c r="B813" t="inlineStr"/>
-      <c r="C813" t="inlineStr"/>
-      <c r="D813" t="inlineStr"/>
+      <c r="B813" t="inlineStr">
+        <is>
+          <t>Paul Jabez Talakayala</t>
+        </is>
+      </c>
+      <c r="C813" t="inlineStr">
+        <is>
+          <t>t.pauljabez@gmail.com</t>
+        </is>
+      </c>
+      <c r="D813" t="inlineStr">
+        <is>
+          <t>ISRAEL</t>
+        </is>
+      </c>
       <c r="E813" t="inlineStr">
         <is>
           <t>526975</t>
@@ -12649,9 +13345,21 @@
           <t>SC015</t>
         </is>
       </c>
-      <c r="B815" t="inlineStr"/>
-      <c r="C815" t="inlineStr"/>
-      <c r="D815" t="inlineStr"/>
+      <c r="B815" t="inlineStr">
+        <is>
+          <t>Koshal Ram</t>
+        </is>
+      </c>
+      <c r="C815" t="inlineStr">
+        <is>
+          <t>koshalram789@gmail.com</t>
+        </is>
+      </c>
+      <c r="D815" t="inlineStr">
+        <is>
+          <t>Russian Federation</t>
+        </is>
+      </c>
       <c r="E815" t="inlineStr">
         <is>
           <t>691799</t>
@@ -15439,9 +16147,21 @@
           <t>SC201</t>
         </is>
       </c>
-      <c r="B1001" t="inlineStr"/>
-      <c r="C1001" t="inlineStr"/>
-      <c r="D1001" t="inlineStr"/>
+      <c r="B1001" t="inlineStr">
+        <is>
+          <t>Alden D'Souza</t>
+        </is>
+      </c>
+      <c r="C1001" t="inlineStr">
+        <is>
+          <t>alden.dsouza@law.christuniversity.in</t>
+        </is>
+      </c>
+      <c r="D1001" t="inlineStr">
+        <is>
+          <t>United States of America</t>
+        </is>
+      </c>
       <c r="E1001" t="inlineStr">
         <is>
           <t>678613</t>
@@ -15484,9 +16204,21 @@
           <t>SC204</t>
         </is>
       </c>
-      <c r="B1004" t="inlineStr"/>
-      <c r="C1004" t="inlineStr"/>
-      <c r="D1004" t="inlineStr"/>
+      <c r="B1004" t="inlineStr">
+        <is>
+          <t>Jyotsna K</t>
+        </is>
+      </c>
+      <c r="C1004" t="inlineStr">
+        <is>
+          <t>sunshine18031965@gmail.com</t>
+        </is>
+      </c>
+      <c r="D1004" t="inlineStr">
+        <is>
+          <t>Mexico</t>
+        </is>
+      </c>
       <c r="E1004" t="inlineStr">
         <is>
           <t>146919</t>
@@ -15499,9 +16231,21 @@
           <t>SC205</t>
         </is>
       </c>
-      <c r="B1005" t="inlineStr"/>
-      <c r="C1005" t="inlineStr"/>
-      <c r="D1005" t="inlineStr"/>
+      <c r="B1005" t="inlineStr">
+        <is>
+          <t>Karthikay Singhal</t>
+        </is>
+      </c>
+      <c r="C1005" t="inlineStr">
+        <is>
+          <t>20jgls-ksinghal@jgu.edu.in</t>
+        </is>
+      </c>
+      <c r="D1005" t="inlineStr">
+        <is>
+          <t>Saint Vincent and the Grenadines</t>
+        </is>
+      </c>
       <c r="E1005" t="inlineStr">
         <is>
           <t>630899</t>
@@ -15514,9 +16258,21 @@
           <t>SC206</t>
         </is>
       </c>
-      <c r="B1006" t="inlineStr"/>
-      <c r="C1006" t="inlineStr"/>
-      <c r="D1006" t="inlineStr"/>
+      <c r="B1006" t="inlineStr">
+        <is>
+          <t>Aditya Chandrashekar</t>
+        </is>
+      </c>
+      <c r="C1006" t="inlineStr">
+        <is>
+          <t>adichandrashekar36@gmail.com</t>
+        </is>
+      </c>
+      <c r="D1006" t="inlineStr">
+        <is>
+          <t>Armenia(O)</t>
+        </is>
+      </c>
       <c r="E1006" t="inlineStr">
         <is>
           <t>987668</t>
@@ -15544,9 +16300,21 @@
           <t>SC208</t>
         </is>
       </c>
-      <c r="B1008" t="inlineStr"/>
-      <c r="C1008" t="inlineStr"/>
-      <c r="D1008" t="inlineStr"/>
+      <c r="B1008" t="inlineStr">
+        <is>
+          <t>Skanda N Magal</t>
+        </is>
+      </c>
+      <c r="C1008" t="inlineStr">
+        <is>
+          <t>skanda905@gmail.com</t>
+        </is>
+      </c>
+      <c r="D1008" t="inlineStr">
+        <is>
+          <t>India</t>
+        </is>
+      </c>
       <c r="E1008" t="inlineStr">
         <is>
           <t>458555</t>
@@ -15574,9 +16342,21 @@
           <t>SC210</t>
         </is>
       </c>
-      <c r="B1010" t="inlineStr"/>
-      <c r="C1010" t="inlineStr"/>
-      <c r="D1010" t="inlineStr"/>
+      <c r="B1010" t="inlineStr">
+        <is>
+          <t>Kiriti Kapavari</t>
+        </is>
+      </c>
+      <c r="C1010" t="inlineStr">
+        <is>
+          <t>forgot02@gmail.com</t>
+        </is>
+      </c>
+      <c r="D1010" t="inlineStr">
+        <is>
+          <t>French Republic</t>
+        </is>
+      </c>
       <c r="E1010" t="inlineStr">
         <is>
           <t>239169</t>
@@ -22954,9 +23734,21 @@
           <t>SC702</t>
         </is>
       </c>
-      <c r="B1502" t="inlineStr"/>
-      <c r="C1502" t="inlineStr"/>
-      <c r="D1502" t="inlineStr"/>
+      <c r="B1502" t="inlineStr">
+        <is>
+          <t>Harshkaran Singh</t>
+        </is>
+      </c>
+      <c r="C1502" t="inlineStr">
+        <is>
+          <t>harsh.karan.singh.09@gmail.com</t>
+        </is>
+      </c>
+      <c r="D1502" t="inlineStr">
+        <is>
+          <t>International Press 1</t>
+        </is>
+      </c>
       <c r="E1502" t="inlineStr">
         <is>
           <t>784371</t>
@@ -23059,9 +23851,21 @@
           <t>SC709</t>
         </is>
       </c>
-      <c r="B1509" t="inlineStr"/>
-      <c r="C1509" t="inlineStr"/>
-      <c r="D1509" t="inlineStr"/>
+      <c r="B1509" t="inlineStr">
+        <is>
+          <t>Sumisha Mohan</t>
+        </is>
+      </c>
+      <c r="C1509" t="inlineStr">
+        <is>
+          <t>sumisha4@gmail.com</t>
+        </is>
+      </c>
+      <c r="D1509" t="inlineStr">
+        <is>
+          <t>International Press 2</t>
+        </is>
+      </c>
       <c r="E1509" t="inlineStr">
         <is>
           <t>794413</t>
@@ -24424,9 +25228,21 @@
           <t>SF001</t>
         </is>
       </c>
-      <c r="B1600" t="inlineStr"/>
-      <c r="C1600" t="inlineStr"/>
-      <c r="D1600" t="inlineStr"/>
+      <c r="B1600" t="inlineStr">
+        <is>
+          <t>Sudhehan Kaliamurthi</t>
+        </is>
+      </c>
+      <c r="C1600" t="inlineStr">
+        <is>
+          <t>sudhe3005@gmail.com</t>
+        </is>
+      </c>
+      <c r="D1600" t="inlineStr">
+        <is>
+          <t>Belgium</t>
+        </is>
+      </c>
       <c r="E1600" t="inlineStr">
         <is>
           <t>262481</t>
@@ -24454,9 +25270,21 @@
           <t>SF003</t>
         </is>
       </c>
-      <c r="B1602" t="inlineStr"/>
-      <c r="C1602" t="inlineStr"/>
-      <c r="D1602" t="inlineStr"/>
+      <c r="B1602" t="inlineStr">
+        <is>
+          <t>Pradeep Vasu</t>
+        </is>
+      </c>
+      <c r="C1602" t="inlineStr">
+        <is>
+          <t>pradeep.arjun96@live.com</t>
+        </is>
+      </c>
+      <c r="D1602" t="inlineStr">
+        <is>
+          <t>CHINA</t>
+        </is>
+      </c>
       <c r="E1602" t="inlineStr">
         <is>
           <t>302665</t>
@@ -24469,9 +25297,21 @@
           <t>SF004</t>
         </is>
       </c>
-      <c r="B1603" t="inlineStr"/>
-      <c r="C1603" t="inlineStr"/>
-      <c r="D1603" t="inlineStr"/>
+      <c r="B1603" t="inlineStr">
+        <is>
+          <t>Rethnakumar Rg</t>
+        </is>
+      </c>
+      <c r="C1603" t="inlineStr">
+        <is>
+          <t>rethnakumar2010010@ssn.edu.in</t>
+        </is>
+      </c>
+      <c r="D1603" t="inlineStr">
+        <is>
+          <t>Cuba</t>
+        </is>
+      </c>
       <c r="E1603" t="inlineStr">
         <is>
           <t>848901</t>
@@ -24484,9 +25324,21 @@
           <t>SF005</t>
         </is>
       </c>
-      <c r="B1604" t="inlineStr"/>
-      <c r="C1604" t="inlineStr"/>
-      <c r="D1604" t="inlineStr"/>
+      <c r="B1604" t="inlineStr">
+        <is>
+          <t>SHRUTHI SUBRAMANI</t>
+        </is>
+      </c>
+      <c r="C1604" t="inlineStr">
+        <is>
+          <t>shruthi2010394@ssn.edu.in</t>
+        </is>
+      </c>
+      <c r="D1604" t="inlineStr">
+        <is>
+          <t>Djibouti</t>
+        </is>
+      </c>
       <c r="E1604" t="inlineStr">
         <is>
           <t>784392</t>
@@ -24499,9 +25351,21 @@
           <t>SF006</t>
         </is>
       </c>
-      <c r="B1605" t="inlineStr"/>
-      <c r="C1605" t="inlineStr"/>
-      <c r="D1605" t="inlineStr"/>
+      <c r="B1605" t="inlineStr">
+        <is>
+          <t>Nabeela Gulam Khader</t>
+        </is>
+      </c>
+      <c r="C1605" t="inlineStr">
+        <is>
+          <t>nabeelakhader27@gmail.com</t>
+        </is>
+      </c>
+      <c r="D1605" t="inlineStr">
+        <is>
+          <t>Finland</t>
+        </is>
+      </c>
       <c r="E1605" t="inlineStr">
         <is>
           <t>498420</t>
@@ -24529,9 +25393,21 @@
           <t>SF008</t>
         </is>
       </c>
-      <c r="B1607" t="inlineStr"/>
-      <c r="C1607" t="inlineStr"/>
-      <c r="D1607" t="inlineStr"/>
+      <c r="B1607" t="inlineStr">
+        <is>
+          <t>Raghav Dinesh</t>
+        </is>
+      </c>
+      <c r="C1607" t="inlineStr">
+        <is>
+          <t>raghavpdinesh@gmail.com</t>
+        </is>
+      </c>
+      <c r="D1607" t="inlineStr">
+        <is>
+          <t>Greece</t>
+        </is>
+      </c>
       <c r="E1607" t="inlineStr">
         <is>
           <t>559295</t>
@@ -24544,9 +25420,21 @@
           <t>SF009</t>
         </is>
       </c>
-      <c r="B1608" t="inlineStr"/>
-      <c r="C1608" t="inlineStr"/>
-      <c r="D1608" t="inlineStr"/>
+      <c r="B1608" t="inlineStr">
+        <is>
+          <t>Thrisha</t>
+        </is>
+      </c>
+      <c r="C1608" t="inlineStr">
+        <is>
+          <t>shrithrisha2010825@ssn.edu.in</t>
+        </is>
+      </c>
+      <c r="D1608" t="inlineStr">
+        <is>
+          <t>Haiti</t>
+        </is>
+      </c>
       <c r="E1608" t="inlineStr">
         <is>
           <t>444933</t>
@@ -24559,9 +25447,21 @@
           <t>SF010</t>
         </is>
       </c>
-      <c r="B1609" t="inlineStr"/>
-      <c r="C1609" t="inlineStr"/>
-      <c r="D1609" t="inlineStr"/>
+      <c r="B1609" t="inlineStr">
+        <is>
+          <t>Keerthana Shankar</t>
+        </is>
+      </c>
+      <c r="C1609" t="inlineStr">
+        <is>
+          <t>pranavdinesan@gmail.com</t>
+        </is>
+      </c>
+      <c r="D1609" t="inlineStr">
+        <is>
+          <t>India</t>
+        </is>
+      </c>
       <c r="E1609" t="inlineStr">
         <is>
           <t>182967</t>
@@ -24574,9 +25474,21 @@
           <t>SF011</t>
         </is>
       </c>
-      <c r="B1610" t="inlineStr"/>
-      <c r="C1610" t="inlineStr"/>
-      <c r="D1610" t="inlineStr"/>
+      <c r="B1610" t="inlineStr">
+        <is>
+          <t>Udit Samant</t>
+        </is>
+      </c>
+      <c r="C1610" t="inlineStr">
+        <is>
+          <t>udit.samant@gmail.com</t>
+        </is>
+      </c>
+      <c r="D1610" t="inlineStr">
+        <is>
+          <t>Italy</t>
+        </is>
+      </c>
       <c r="E1610" t="inlineStr">
         <is>
           <t>840770</t>
@@ -24589,9 +25501,21 @@
           <t>SF012</t>
         </is>
       </c>
-      <c r="B1611" t="inlineStr"/>
-      <c r="C1611" t="inlineStr"/>
-      <c r="D1611" t="inlineStr"/>
+      <c r="B1611" t="inlineStr">
+        <is>
+          <t>Sivaram E</t>
+        </is>
+      </c>
+      <c r="C1611" t="inlineStr">
+        <is>
+          <t>sivaramelumalai4032588@gmail.com</t>
+        </is>
+      </c>
+      <c r="D1611" t="inlineStr">
+        <is>
+          <t>Japan</t>
+        </is>
+      </c>
       <c r="E1611" t="inlineStr">
         <is>
           <t>147645</t>
@@ -24604,9 +25528,21 @@
           <t>SF013</t>
         </is>
       </c>
-      <c r="B1612" t="inlineStr"/>
-      <c r="C1612" t="inlineStr"/>
-      <c r="D1612" t="inlineStr"/>
+      <c r="B1612" t="inlineStr">
+        <is>
+          <t>Vignesh M</t>
+        </is>
+      </c>
+      <c r="C1612" t="inlineStr">
+        <is>
+          <t>vignesh2010587@ssn.edu.in</t>
+        </is>
+      </c>
+      <c r="D1612" t="inlineStr">
+        <is>
+          <t>Kiribati</t>
+        </is>
+      </c>
       <c r="E1612" t="inlineStr">
         <is>
           <t>700504</t>
@@ -24634,9 +25570,21 @@
           <t>SF015</t>
         </is>
       </c>
-      <c r="B1614" t="inlineStr"/>
-      <c r="C1614" t="inlineStr"/>
-      <c r="D1614" t="inlineStr"/>
+      <c r="B1614" t="inlineStr">
+        <is>
+          <t>Syed Thaha Osman</t>
+        </is>
+      </c>
+      <c r="C1614" t="inlineStr">
+        <is>
+          <t>syedthaha969@gmail.com</t>
+        </is>
+      </c>
+      <c r="D1614" t="inlineStr">
+        <is>
+          <t>Mexico</t>
+        </is>
+      </c>
       <c r="E1614" t="inlineStr">
         <is>
           <t>152946</t>
@@ -24649,9 +25597,21 @@
           <t>SF016</t>
         </is>
       </c>
-      <c r="B1615" t="inlineStr"/>
-      <c r="C1615" t="inlineStr"/>
-      <c r="D1615" t="inlineStr"/>
+      <c r="B1615" t="inlineStr">
+        <is>
+          <t>Bhagavathi R</t>
+        </is>
+      </c>
+      <c r="C1615" t="inlineStr">
+        <is>
+          <t>bhagavathir9@gmail.com</t>
+        </is>
+      </c>
+      <c r="D1615" t="inlineStr">
+        <is>
+          <t>New Zealand</t>
+        </is>
+      </c>
       <c r="E1615" t="inlineStr">
         <is>
           <t>827970</t>
@@ -24664,9 +25624,21 @@
           <t>SF017</t>
         </is>
       </c>
-      <c r="B1616" t="inlineStr"/>
-      <c r="C1616" t="inlineStr"/>
-      <c r="D1616" t="inlineStr"/>
+      <c r="B1616" t="inlineStr">
+        <is>
+          <t>Nandakishor V</t>
+        </is>
+      </c>
+      <c r="C1616" t="inlineStr">
+        <is>
+          <t>nandhu21velu@gmail.com</t>
+        </is>
+      </c>
+      <c r="D1616" t="inlineStr">
+        <is>
+          <t>Qatar</t>
+        </is>
+      </c>
       <c r="E1616" t="inlineStr">
         <is>
           <t>857986</t>
@@ -24679,9 +25651,21 @@
           <t>SF018</t>
         </is>
       </c>
-      <c r="B1617" t="inlineStr"/>
-      <c r="C1617" t="inlineStr"/>
-      <c r="D1617" t="inlineStr"/>
+      <c r="B1617" t="inlineStr">
+        <is>
+          <t>GR Pavan</t>
+        </is>
+      </c>
+      <c r="C1617" t="inlineStr">
+        <is>
+          <t>grpavan0705@gmail.com</t>
+        </is>
+      </c>
+      <c r="D1617" t="inlineStr">
+        <is>
+          <t>Singapore</t>
+        </is>
+      </c>
       <c r="E1617" t="inlineStr">
         <is>
           <t>775068</t>
@@ -24724,9 +25708,21 @@
           <t>SF021</t>
         </is>
       </c>
-      <c r="B1620" t="inlineStr"/>
-      <c r="C1620" t="inlineStr"/>
-      <c r="D1620" t="inlineStr"/>
+      <c r="B1620" t="inlineStr">
+        <is>
+          <t>E Nivetha</t>
+        </is>
+      </c>
+      <c r="C1620" t="inlineStr">
+        <is>
+          <t>nivetha2010668@ssn.edu.in</t>
+        </is>
+      </c>
+      <c r="D1620" t="inlineStr">
+        <is>
+          <t>Sweden</t>
+        </is>
+      </c>
       <c r="E1620" t="inlineStr">
         <is>
           <t>445194</t>
@@ -24739,9 +25735,21 @@
           <t>SF022</t>
         </is>
       </c>
-      <c r="B1621" t="inlineStr"/>
-      <c r="C1621" t="inlineStr"/>
-      <c r="D1621" t="inlineStr"/>
+      <c r="B1621" t="inlineStr">
+        <is>
+          <t>M Chellakkamar</t>
+        </is>
+      </c>
+      <c r="C1621" t="inlineStr">
+        <is>
+          <t>chellakkumar77@gmail.com</t>
+        </is>
+      </c>
+      <c r="D1621" t="inlineStr">
+        <is>
+          <t>Taiwan</t>
+        </is>
+      </c>
       <c r="E1621" t="inlineStr">
         <is>
           <t>013636</t>
@@ -24769,9 +25777,21 @@
           <t>SF024</t>
         </is>
       </c>
-      <c r="B1623" t="inlineStr"/>
-      <c r="C1623" t="inlineStr"/>
-      <c r="D1623" t="inlineStr"/>
+      <c r="B1623" t="inlineStr">
+        <is>
+          <t>Shivangi Pandey</t>
+        </is>
+      </c>
+      <c r="C1623" t="inlineStr">
+        <is>
+          <t>shivangi1950@bme.ssn.edu.in</t>
+        </is>
+      </c>
+      <c r="D1623" t="inlineStr">
+        <is>
+          <t>Turkey</t>
+        </is>
+      </c>
       <c r="E1623" t="inlineStr">
         <is>
           <t>923843</t>
@@ -24784,9 +25804,21 @@
           <t>SF025</t>
         </is>
       </c>
-      <c r="B1624" t="inlineStr"/>
-      <c r="C1624" t="inlineStr"/>
-      <c r="D1624" t="inlineStr"/>
+      <c r="B1624" t="inlineStr">
+        <is>
+          <t>Supraja Vaidhyanathan</t>
+        </is>
+      </c>
+      <c r="C1624" t="inlineStr">
+        <is>
+          <t>bhama26@gmail.com</t>
+        </is>
+      </c>
+      <c r="D1624" t="inlineStr">
+        <is>
+          <t>United Arab Emirates</t>
+        </is>
+      </c>
       <c r="E1624" t="inlineStr">
         <is>
           <t>867216</t>
@@ -24799,9 +25831,21 @@
           <t>SF026</t>
         </is>
       </c>
-      <c r="B1625" t="inlineStr"/>
-      <c r="C1625" t="inlineStr"/>
-      <c r="D1625" t="inlineStr"/>
+      <c r="B1625" t="inlineStr">
+        <is>
+          <t>Hrishikesh Kumar</t>
+        </is>
+      </c>
+      <c r="C1625" t="inlineStr">
+        <is>
+          <t>hrishikesh.kumar28@gmail.com</t>
+        </is>
+      </c>
+      <c r="D1625" t="inlineStr">
+        <is>
+          <t>Zimbabwe</t>
+        </is>
+      </c>
       <c r="E1625" t="inlineStr">
         <is>
           <t>312212</t>
@@ -25969,9 +27013,21 @@
           <t>SF104</t>
         </is>
       </c>
-      <c r="B1703" t="inlineStr"/>
-      <c r="C1703" t="inlineStr"/>
-      <c r="D1703" t="inlineStr"/>
+      <c r="B1703" t="inlineStr">
+        <is>
+          <t>Adrij A Mohan</t>
+        </is>
+      </c>
+      <c r="C1703" t="inlineStr">
+        <is>
+          <t>adrijmohan.0901@gmail.com</t>
+        </is>
+      </c>
+      <c r="D1703" t="inlineStr">
+        <is>
+          <t>Canada</t>
+        </is>
+      </c>
       <c r="E1703" t="inlineStr">
         <is>
           <t>543607</t>
@@ -26014,9 +27070,21 @@
           <t>SF107</t>
         </is>
       </c>
-      <c r="B1706" t="inlineStr"/>
-      <c r="C1706" t="inlineStr"/>
-      <c r="D1706" t="inlineStr"/>
+      <c r="B1706" t="inlineStr">
+        <is>
+          <t>Vishal Venkatarangan</t>
+        </is>
+      </c>
+      <c r="C1706" t="inlineStr">
+        <is>
+          <t>vishalvenkat33@gmail.com</t>
+        </is>
+      </c>
+      <c r="D1706" t="inlineStr">
+        <is>
+          <t>Germany</t>
+        </is>
+      </c>
       <c r="E1706" t="inlineStr">
         <is>
           <t>069392</t>
@@ -26029,9 +27097,21 @@
           <t>SF108</t>
         </is>
       </c>
-      <c r="B1707" t="inlineStr"/>
-      <c r="C1707" t="inlineStr"/>
-      <c r="D1707" t="inlineStr"/>
+      <c r="B1707" t="inlineStr">
+        <is>
+          <t>Nishtha L</t>
+        </is>
+      </c>
+      <c r="C1707" t="inlineStr">
+        <is>
+          <t>125117031@sastra.ac.in</t>
+        </is>
+      </c>
+      <c r="D1707" t="inlineStr">
+        <is>
+          <t>Libya</t>
+        </is>
+      </c>
       <c r="E1707" t="inlineStr">
         <is>
           <t>490144</t>
@@ -26059,9 +27139,21 @@
           <t>SF110</t>
         </is>
       </c>
-      <c r="B1709" t="inlineStr"/>
-      <c r="C1709" t="inlineStr"/>
-      <c r="D1709" t="inlineStr"/>
+      <c r="B1709" t="inlineStr">
+        <is>
+          <t>Priyanka Balu</t>
+        </is>
+      </c>
+      <c r="C1709" t="inlineStr">
+        <is>
+          <t>balu2010850@ssn.edu.in</t>
+        </is>
+      </c>
+      <c r="D1709" t="inlineStr">
+        <is>
+          <t>Malaysia</t>
+        </is>
+      </c>
       <c r="E1709" t="inlineStr">
         <is>
           <t>473324</t>
@@ -26104,9 +27196,21 @@
           <t>SF113</t>
         </is>
       </c>
-      <c r="B1712" t="inlineStr"/>
-      <c r="C1712" t="inlineStr"/>
-      <c r="D1712" t="inlineStr"/>
+      <c r="B1712" t="inlineStr">
+        <is>
+          <t>K.V. Vaishnave</t>
+        </is>
+      </c>
+      <c r="C1712" t="inlineStr">
+        <is>
+          <t>vaishnave.arul@gmail.com</t>
+        </is>
+      </c>
+      <c r="D1712" t="inlineStr">
+        <is>
+          <t>Nicaragua</t>
+        </is>
+      </c>
       <c r="E1712" t="inlineStr">
         <is>
           <t>817177</t>
@@ -26119,9 +27223,21 @@
           <t>SF114</t>
         </is>
       </c>
-      <c r="B1713" t="inlineStr"/>
-      <c r="C1713" t="inlineStr"/>
-      <c r="D1713" t="inlineStr"/>
+      <c r="B1713" t="inlineStr">
+        <is>
+          <t>Hariharasubramanyam KM</t>
+        </is>
+      </c>
+      <c r="C1713" t="inlineStr">
+        <is>
+          <t>kmhari2002@gmail.com</t>
+        </is>
+      </c>
+      <c r="D1713" t="inlineStr">
+        <is>
+          <t>Pakistan</t>
+        </is>
+      </c>
       <c r="E1713" t="inlineStr">
         <is>
           <t>410685</t>
@@ -26134,9 +27250,21 @@
           <t>SF115</t>
         </is>
       </c>
-      <c r="B1714" t="inlineStr"/>
-      <c r="C1714" t="inlineStr"/>
-      <c r="D1714" t="inlineStr"/>
+      <c r="B1714" t="inlineStr">
+        <is>
+          <t>Dhanush Gajaraj</t>
+        </is>
+      </c>
+      <c r="C1714" t="inlineStr">
+        <is>
+          <t>dhanushdhoni15@gmail.com</t>
+        </is>
+      </c>
+      <c r="D1714" t="inlineStr">
+        <is>
+          <t>Portugal</t>
+        </is>
+      </c>
       <c r="E1714" t="inlineStr">
         <is>
           <t>262379</t>
@@ -26149,9 +27277,21 @@
           <t>SF116</t>
         </is>
       </c>
-      <c r="B1715" t="inlineStr"/>
-      <c r="C1715" t="inlineStr"/>
-      <c r="D1715" t="inlineStr"/>
+      <c r="B1715" t="inlineStr">
+        <is>
+          <t>Vandhana R</t>
+        </is>
+      </c>
+      <c r="C1715" t="inlineStr">
+        <is>
+          <t>officialvandy@gmail.com</t>
+        </is>
+      </c>
+      <c r="D1715" t="inlineStr">
+        <is>
+          <t>Russia</t>
+        </is>
+      </c>
       <c r="E1715" t="inlineStr">
         <is>
           <t>251739</t>
@@ -26164,9 +27304,21 @@
           <t>SF117</t>
         </is>
       </c>
-      <c r="B1716" t="inlineStr"/>
-      <c r="C1716" t="inlineStr"/>
-      <c r="D1716" t="inlineStr"/>
+      <c r="B1716" t="inlineStr">
+        <is>
+          <t>Malaveka A</t>
+        </is>
+      </c>
+      <c r="C1716" t="inlineStr">
+        <is>
+          <t>amalaveka@gmail.com</t>
+        </is>
+      </c>
+      <c r="D1716" t="inlineStr">
+        <is>
+          <t>Rwanda</t>
+        </is>
+      </c>
       <c r="E1716" t="inlineStr">
         <is>
           <t>529735</t>
@@ -26209,9 +27361,21 @@
           <t>SF120</t>
         </is>
       </c>
-      <c r="B1719" t="inlineStr"/>
-      <c r="C1719" t="inlineStr"/>
-      <c r="D1719" t="inlineStr"/>
+      <c r="B1719" t="inlineStr">
+        <is>
+          <t>Abhishek P.S.</t>
+        </is>
+      </c>
+      <c r="C1719" t="inlineStr">
+        <is>
+          <t>abishek05072004@gmail.com</t>
+        </is>
+      </c>
+      <c r="D1719" t="inlineStr">
+        <is>
+          <t>Sierra Leone</t>
+        </is>
+      </c>
       <c r="E1719" t="inlineStr">
         <is>
           <t>217635</t>
@@ -26269,9 +27433,21 @@
           <t>SF124</t>
         </is>
       </c>
-      <c r="B1723" t="inlineStr"/>
-      <c r="C1723" t="inlineStr"/>
-      <c r="D1723" t="inlineStr"/>
+      <c r="B1723" t="inlineStr">
+        <is>
+          <t>Aditya Kumar</t>
+        </is>
+      </c>
+      <c r="C1723" t="inlineStr">
+        <is>
+          <t>adi_kumar02@yahoo.com</t>
+        </is>
+      </c>
+      <c r="D1723" t="inlineStr">
+        <is>
+          <t>Switzerland</t>
+        </is>
+      </c>
       <c r="E1723" t="inlineStr">
         <is>
           <t>786295</t>
@@ -26299,9 +27475,21 @@
           <t>SF126</t>
         </is>
       </c>
-      <c r="B1725" t="inlineStr"/>
-      <c r="C1725" t="inlineStr"/>
-      <c r="D1725" t="inlineStr"/>
+      <c r="B1725" t="inlineStr">
+        <is>
+          <t>Pooja Kalyan Kumar</t>
+        </is>
+      </c>
+      <c r="C1725" t="inlineStr">
+        <is>
+          <t>nilakalyan.asg@gmail.com</t>
+        </is>
+      </c>
+      <c r="D1725" t="inlineStr">
+        <is>
+          <t>Tunisia</t>
+        </is>
+      </c>
       <c r="E1725" t="inlineStr">
         <is>
           <t>144723</t>
@@ -27424,9 +28612,21 @@
           <t>SF201</t>
         </is>
       </c>
-      <c r="B1800" t="inlineStr"/>
-      <c r="C1800" t="inlineStr"/>
-      <c r="D1800" t="inlineStr"/>
+      <c r="B1800" t="inlineStr">
+        <is>
+          <t>Sakshi Puri</t>
+        </is>
+      </c>
+      <c r="C1800" t="inlineStr">
+        <is>
+          <t>sakshipuri007@gmail.com</t>
+        </is>
+      </c>
+      <c r="D1800" t="inlineStr">
+        <is>
+          <t>Australia</t>
+        </is>
+      </c>
       <c r="E1800" t="inlineStr">
         <is>
           <t>220754</t>
@@ -27454,9 +28654,21 @@
           <t>SF203</t>
         </is>
       </c>
-      <c r="B1802" t="inlineStr"/>
-      <c r="C1802" t="inlineStr"/>
-      <c r="D1802" t="inlineStr"/>
+      <c r="B1802" t="inlineStr">
+        <is>
+          <t>Anjali Saran</t>
+        </is>
+      </c>
+      <c r="C1802" t="inlineStr">
+        <is>
+          <t>anjali.saran@law.christuniversity.in</t>
+        </is>
+      </c>
+      <c r="D1802" t="inlineStr">
+        <is>
+          <t>Egypt</t>
+        </is>
+      </c>
       <c r="E1802" t="inlineStr">
         <is>
           <t>606930</t>
@@ -27469,9 +28681,21 @@
           <t>SF204</t>
         </is>
       </c>
-      <c r="B1803" t="inlineStr"/>
-      <c r="C1803" t="inlineStr"/>
-      <c r="D1803" t="inlineStr"/>
+      <c r="B1803" t="inlineStr">
+        <is>
+          <t>Madhuri Mahalingam</t>
+        </is>
+      </c>
+      <c r="C1803" t="inlineStr">
+        <is>
+          <t>madhurimaha2405@gmail.com</t>
+        </is>
+      </c>
+      <c r="D1803" t="inlineStr">
+        <is>
+          <t>France</t>
+        </is>
+      </c>
       <c r="E1803" t="inlineStr">
         <is>
           <t>642301</t>
@@ -27484,9 +28708,21 @@
           <t>SF205</t>
         </is>
       </c>
-      <c r="B1804" t="inlineStr"/>
-      <c r="C1804" t="inlineStr"/>
-      <c r="D1804" t="inlineStr"/>
+      <c r="B1804" t="inlineStr">
+        <is>
+          <t>Izma Zainab</t>
+        </is>
+      </c>
+      <c r="C1804" t="inlineStr">
+        <is>
+          <t>izmazainab@gmail.com</t>
+        </is>
+      </c>
+      <c r="D1804" t="inlineStr">
+        <is>
+          <t>Ghana</t>
+        </is>
+      </c>
       <c r="E1804" t="inlineStr">
         <is>
           <t>085978</t>
@@ -27514,9 +28750,21 @@
           <t>SF207</t>
         </is>
       </c>
-      <c r="B1806" t="inlineStr"/>
-      <c r="C1806" t="inlineStr"/>
-      <c r="D1806" t="inlineStr"/>
+      <c r="B1806" t="inlineStr">
+        <is>
+          <t>Chinmayee Dindore</t>
+        </is>
+      </c>
+      <c r="C1806" t="inlineStr">
+        <is>
+          <t>chinmayee.dindorez13@gmail.com</t>
+        </is>
+      </c>
+      <c r="D1806" t="inlineStr">
+        <is>
+          <t>Netherlands</t>
+        </is>
+      </c>
       <c r="E1806" t="inlineStr">
         <is>
           <t>338300</t>
@@ -27589,9 +28837,21 @@
           <t>SF212</t>
         </is>
       </c>
-      <c r="B1811" t="inlineStr"/>
-      <c r="C1811" t="inlineStr"/>
-      <c r="D1811" t="inlineStr"/>
+      <c r="B1811" t="inlineStr">
+        <is>
+          <t>Kommu Sreeraj</t>
+        </is>
+      </c>
+      <c r="C1811" t="inlineStr">
+        <is>
+          <t>sreerajkommu38@gmail.com</t>
+        </is>
+      </c>
+      <c r="D1811" t="inlineStr">
+        <is>
+          <t>Brazil</t>
+        </is>
+      </c>
       <c r="E1811" t="inlineStr">
         <is>
           <t>206789</t>
@@ -27604,9 +28864,21 @@
           <t>SF213</t>
         </is>
       </c>
-      <c r="B1812" t="inlineStr"/>
-      <c r="C1812" t="inlineStr"/>
-      <c r="D1812" t="inlineStr"/>
+      <c r="B1812" t="inlineStr">
+        <is>
+          <t>Bhavya Kandhari</t>
+        </is>
+      </c>
+      <c r="C1812" t="inlineStr">
+        <is>
+          <t>bhavya_k.sias20@krea.ac.in</t>
+        </is>
+      </c>
+      <c r="D1812" t="inlineStr">
+        <is>
+          <t>United Kingdom</t>
+        </is>
+      </c>
       <c r="E1812" t="inlineStr">
         <is>
           <t>725490</t>
@@ -27619,9 +28891,21 @@
           <t>SF214</t>
         </is>
       </c>
-      <c r="B1813" t="inlineStr"/>
-      <c r="C1813" t="inlineStr"/>
-      <c r="D1813" t="inlineStr"/>
+      <c r="B1813" t="inlineStr">
+        <is>
+          <t>Domil Antony Johnson</t>
+        </is>
+      </c>
+      <c r="C1813" t="inlineStr">
+        <is>
+          <t>imdomilantonyjohnson18@gmail.com</t>
+        </is>
+      </c>
+      <c r="D1813" t="inlineStr">
+        <is>
+          <t>United States of America</t>
+        </is>
+      </c>
       <c r="E1813" t="inlineStr">
         <is>
           <t>598316</t>
@@ -32734,9 +34018,21 @@
           <t>SF555</t>
         </is>
       </c>
-      <c r="B2154" t="inlineStr"/>
-      <c r="C2154" t="inlineStr"/>
-      <c r="D2154" t="inlineStr"/>
+      <c r="B2154" t="inlineStr">
+        <is>
+          <t>Gokul Krishna</t>
+        </is>
+      </c>
+      <c r="C2154" t="inlineStr">
+        <is>
+          <t>kampalagokul@gmail.com</t>
+        </is>
+      </c>
+      <c r="D2154" t="inlineStr">
+        <is>
+          <t>Somalia</t>
+        </is>
+      </c>
       <c r="E2154" t="inlineStr">
         <is>
           <t>558822</t>
@@ -34969,9 +36265,21 @@
           <t>SF704</t>
         </is>
       </c>
-      <c r="B2303" t="inlineStr"/>
-      <c r="C2303" t="inlineStr"/>
-      <c r="D2303" t="inlineStr"/>
+      <c r="B2303" t="inlineStr">
+        <is>
+          <t>Surya Sridhar</t>
+        </is>
+      </c>
+      <c r="C2303" t="inlineStr">
+        <is>
+          <t>surya.sridhar.20127@gmail.com</t>
+        </is>
+      </c>
+      <c r="D2303" t="inlineStr">
+        <is>
+          <t>International Press 1</t>
+        </is>
+      </c>
       <c r="E2303" t="inlineStr">
         <is>
           <t>395725</t>
@@ -34984,9 +36292,21 @@
           <t>SF705</t>
         </is>
       </c>
-      <c r="B2304" t="inlineStr"/>
-      <c r="C2304" t="inlineStr"/>
-      <c r="D2304" t="inlineStr"/>
+      <c r="B2304" t="inlineStr">
+        <is>
+          <t>Aaditya Shankar Natarajan</t>
+        </is>
+      </c>
+      <c r="C2304" t="inlineStr">
+        <is>
+          <t>aaditya.shankar.n@gmail.com</t>
+        </is>
+      </c>
+      <c r="D2304" t="inlineStr">
+        <is>
+          <t>International Press 2</t>
+        </is>
+      </c>
       <c r="E2304" t="inlineStr">
         <is>
           <t>774035</t>
@@ -34999,9 +36319,21 @@
           <t>SF706</t>
         </is>
       </c>
-      <c r="B2305" t="inlineStr"/>
-      <c r="C2305" t="inlineStr"/>
-      <c r="D2305" t="inlineStr"/>
+      <c r="B2305" t="inlineStr">
+        <is>
+          <t>Sakshi Jain</t>
+        </is>
+      </c>
+      <c r="C2305" t="inlineStr">
+        <is>
+          <t>saaku06@gmail.com</t>
+        </is>
+      </c>
+      <c r="D2305" t="inlineStr">
+        <is>
+          <t>International Press 3</t>
+        </is>
+      </c>
       <c r="E2305" t="inlineStr">
         <is>
           <t>850858</t>
@@ -36439,9 +37771,21 @@
           <t>HR003</t>
         </is>
       </c>
-      <c r="B2401" t="inlineStr"/>
-      <c r="C2401" t="inlineStr"/>
-      <c r="D2401" t="inlineStr"/>
+      <c r="B2401" t="inlineStr">
+        <is>
+          <t>Kaarnika Mahendran</t>
+        </is>
+      </c>
+      <c r="C2401" t="inlineStr">
+        <is>
+          <t>kaarnikamalik@gmail.com</t>
+        </is>
+      </c>
+      <c r="D2401" t="inlineStr">
+        <is>
+          <t>Bahamas</t>
+        </is>
+      </c>
       <c r="E2401" t="inlineStr">
         <is>
           <t>058078</t>
@@ -36454,9 +37798,21 @@
           <t>HR004</t>
         </is>
       </c>
-      <c r="B2402" t="inlineStr"/>
-      <c r="C2402" t="inlineStr"/>
-      <c r="D2402" t="inlineStr"/>
+      <c r="B2402" t="inlineStr">
+        <is>
+          <t>Dhivya Shri</t>
+        </is>
+      </c>
+      <c r="C2402" t="inlineStr">
+        <is>
+          <t>dhivyashri4uma@gmail.com</t>
+        </is>
+      </c>
+      <c r="D2402" t="inlineStr">
+        <is>
+          <t>Bahrain</t>
+        </is>
+      </c>
       <c r="E2402" t="inlineStr">
         <is>
           <t>373524</t>
@@ -36484,9 +37840,21 @@
           <t>HR006</t>
         </is>
       </c>
-      <c r="B2404" t="inlineStr"/>
-      <c r="C2404" t="inlineStr"/>
-      <c r="D2404" t="inlineStr"/>
+      <c r="B2404" t="inlineStr">
+        <is>
+          <t>K S RAMALAKSHMI</t>
+        </is>
+      </c>
+      <c r="C2404" t="inlineStr">
+        <is>
+          <t>rlsri2305@gmail.com</t>
+        </is>
+      </c>
+      <c r="D2404" t="inlineStr">
+        <is>
+          <t>Bolivia</t>
+        </is>
+      </c>
       <c r="E2404" t="inlineStr">
         <is>
           <t>820321</t>
@@ -36514,9 +37882,21 @@
           <t>HR008</t>
         </is>
       </c>
-      <c r="B2406" t="inlineStr"/>
-      <c r="C2406" t="inlineStr"/>
-      <c r="D2406" t="inlineStr"/>
+      <c r="B2406" t="inlineStr">
+        <is>
+          <t>Vasundhara Vishnuraj</t>
+        </is>
+      </c>
+      <c r="C2406" t="inlineStr">
+        <is>
+          <t>vandhanavishnuraj27@gmail.com</t>
+        </is>
+      </c>
+      <c r="D2406" t="inlineStr">
+        <is>
+          <t>Bulgaria</t>
+        </is>
+      </c>
       <c r="E2406" t="inlineStr">
         <is>
           <t>468948</t>
@@ -36544,9 +37924,21 @@
           <t>HR010</t>
         </is>
       </c>
-      <c r="B2408" t="inlineStr"/>
-      <c r="C2408" t="inlineStr"/>
-      <c r="D2408" t="inlineStr"/>
+      <c r="B2408" t="inlineStr">
+        <is>
+          <t>Kaushic Aravind B</t>
+        </is>
+      </c>
+      <c r="C2408" t="inlineStr">
+        <is>
+          <t>aspirearavind@gmail.com</t>
+        </is>
+      </c>
+      <c r="D2408" t="inlineStr">
+        <is>
+          <t>China</t>
+        </is>
+      </c>
       <c r="E2408" t="inlineStr">
         <is>
           <t>248662</t>
@@ -36574,9 +37966,21 @@
           <t>HR012</t>
         </is>
       </c>
-      <c r="B2410" t="inlineStr"/>
-      <c r="C2410" t="inlineStr"/>
-      <c r="D2410" t="inlineStr"/>
+      <c r="B2410" t="inlineStr">
+        <is>
+          <t>Varsha sivaramakrishnan</t>
+        </is>
+      </c>
+      <c r="C2410" t="inlineStr">
+        <is>
+          <t>svarshakrishnan@gmail.com</t>
+        </is>
+      </c>
+      <c r="D2410" t="inlineStr">
+        <is>
+          <t>Cuba</t>
+        </is>
+      </c>
       <c r="E2410" t="inlineStr">
         <is>
           <t>922077</t>
@@ -36589,9 +37993,21 @@
           <t>HR013</t>
         </is>
       </c>
-      <c r="B2411" t="inlineStr"/>
-      <c r="C2411" t="inlineStr"/>
-      <c r="D2411" t="inlineStr"/>
+      <c r="B2411" t="inlineStr">
+        <is>
+          <t>T R SRI SUDARSAN</t>
+        </is>
+      </c>
+      <c r="C2411" t="inlineStr">
+        <is>
+          <t>getasri2@gmail.com</t>
+        </is>
+      </c>
+      <c r="D2411" t="inlineStr">
+        <is>
+          <t>Eritrea</t>
+        </is>
+      </c>
       <c r="E2411" t="inlineStr">
         <is>
           <t>778015</t>
@@ -36604,9 +38020,21 @@
           <t>HR014</t>
         </is>
       </c>
-      <c r="B2412" t="inlineStr"/>
-      <c r="C2412" t="inlineStr"/>
-      <c r="D2412" t="inlineStr"/>
+      <c r="B2412" t="inlineStr">
+        <is>
+          <t>Meera Kumar</t>
+        </is>
+      </c>
+      <c r="C2412" t="inlineStr">
+        <is>
+          <t>meerakumaar9@gmail.com</t>
+        </is>
+      </c>
+      <c r="D2412" t="inlineStr">
+        <is>
+          <t>Fiji</t>
+        </is>
+      </c>
       <c r="E2412" t="inlineStr">
         <is>
           <t>396272</t>
@@ -36619,9 +38047,21 @@
           <t>HR015</t>
         </is>
       </c>
-      <c r="B2413" t="inlineStr"/>
-      <c r="C2413" t="inlineStr"/>
-      <c r="D2413" t="inlineStr"/>
+      <c r="B2413" t="inlineStr">
+        <is>
+          <t>Rohith Harikrishnan</t>
+        </is>
+      </c>
+      <c r="C2413" t="inlineStr">
+        <is>
+          <t>rohith.harikrishnan@gmail.com</t>
+        </is>
+      </c>
+      <c r="D2413" t="inlineStr">
+        <is>
+          <t>FRANCE</t>
+        </is>
+      </c>
       <c r="E2413" t="inlineStr">
         <is>
           <t>501115</t>
@@ -36664,9 +38104,21 @@
           <t>HR018</t>
         </is>
       </c>
-      <c r="B2416" t="inlineStr"/>
-      <c r="C2416" t="inlineStr"/>
-      <c r="D2416" t="inlineStr"/>
+      <c r="B2416" t="inlineStr">
+        <is>
+          <t>Shankar Vinayak S</t>
+        </is>
+      </c>
+      <c r="C2416" t="inlineStr">
+        <is>
+          <t>shankarsaroja1998@gmail.com</t>
+        </is>
+      </c>
+      <c r="D2416" t="inlineStr">
+        <is>
+          <t>Italy</t>
+        </is>
+      </c>
       <c r="E2416" t="inlineStr">
         <is>
           <t>823036</t>
@@ -36679,9 +38131,21 @@
           <t>HR019</t>
         </is>
       </c>
-      <c r="B2417" t="inlineStr"/>
-      <c r="C2417" t="inlineStr"/>
-      <c r="D2417" t="inlineStr"/>
+      <c r="B2417" t="inlineStr">
+        <is>
+          <t>Sanjit</t>
+        </is>
+      </c>
+      <c r="C2417" t="inlineStr">
+        <is>
+          <t>sanjitkirankk@gmail.com</t>
+        </is>
+      </c>
+      <c r="D2417" t="inlineStr">
+        <is>
+          <t>MALAWI</t>
+        </is>
+      </c>
       <c r="E2417" t="inlineStr">
         <is>
           <t>223264</t>
@@ -36694,9 +38158,21 @@
           <t>HR020</t>
         </is>
       </c>
-      <c r="B2418" t="inlineStr"/>
-      <c r="C2418" t="inlineStr"/>
-      <c r="D2418" t="inlineStr"/>
+      <c r="B2418" t="inlineStr">
+        <is>
+          <t>K Arjun Bharath</t>
+        </is>
+      </c>
+      <c r="C2418" t="inlineStr">
+        <is>
+          <t>arjunbharath120900@gmail.com</t>
+        </is>
+      </c>
+      <c r="D2418" t="inlineStr">
+        <is>
+          <t>Marshall Islands</t>
+        </is>
+      </c>
       <c r="E2418" t="inlineStr">
         <is>
           <t>683820</t>
@@ -36724,9 +38200,21 @@
           <t>HR022</t>
         </is>
       </c>
-      <c r="B2420" t="inlineStr"/>
-      <c r="C2420" t="inlineStr"/>
-      <c r="D2420" t="inlineStr"/>
+      <c r="B2420" t="inlineStr">
+        <is>
+          <t>Gunanicaa Arun</t>
+        </is>
+      </c>
+      <c r="C2420" t="inlineStr">
+        <is>
+          <t>gunanicaa2010257@ssn.edu.in</t>
+        </is>
+      </c>
+      <c r="D2420" t="inlineStr">
+        <is>
+          <t>MEXICO</t>
+        </is>
+      </c>
       <c r="E2420" t="inlineStr">
         <is>
           <t>862673</t>
@@ -36769,9 +38257,21 @@
           <t>HR025</t>
         </is>
       </c>
-      <c r="B2423" t="inlineStr"/>
-      <c r="C2423" t="inlineStr"/>
-      <c r="D2423" t="inlineStr"/>
+      <c r="B2423" t="inlineStr">
+        <is>
+          <t>Raajameenakshi AL</t>
+        </is>
+      </c>
+      <c r="C2423" t="inlineStr">
+        <is>
+          <t>raajameenakshial@gmail.com</t>
+        </is>
+      </c>
+      <c r="D2423" t="inlineStr">
+        <is>
+          <t>Philippines</t>
+        </is>
+      </c>
       <c r="E2423" t="inlineStr">
         <is>
           <t>350929</t>
@@ -36799,9 +38299,21 @@
           <t>HR027</t>
         </is>
       </c>
-      <c r="B2425" t="inlineStr"/>
-      <c r="C2425" t="inlineStr"/>
-      <c r="D2425" t="inlineStr"/>
+      <c r="B2425" t="inlineStr">
+        <is>
+          <t>Anirudh Ram</t>
+        </is>
+      </c>
+      <c r="C2425" t="inlineStr">
+        <is>
+          <t>anirudhramk@gmail.com</t>
+        </is>
+      </c>
+      <c r="D2425" t="inlineStr">
+        <is>
+          <t>Republic of Korea</t>
+        </is>
+      </c>
       <c r="E2425" t="inlineStr">
         <is>
           <t>128365</t>
@@ -36814,9 +38326,21 @@
           <t>HR028</t>
         </is>
       </c>
-      <c r="B2426" t="inlineStr"/>
-      <c r="C2426" t="inlineStr"/>
-      <c r="D2426" t="inlineStr"/>
+      <c r="B2426" t="inlineStr">
+        <is>
+          <t>Vikash Anand</t>
+        </is>
+      </c>
+      <c r="C2426" t="inlineStr">
+        <is>
+          <t>vikashanand.sasi@gmail.com</t>
+        </is>
+      </c>
+      <c r="D2426" t="inlineStr">
+        <is>
+          <t>Senegal</t>
+        </is>
+      </c>
       <c r="E2426" t="inlineStr">
         <is>
           <t>685506</t>
@@ -36829,9 +38353,21 @@
           <t>HR029</t>
         </is>
       </c>
-      <c r="B2427" t="inlineStr"/>
-      <c r="C2427" t="inlineStr"/>
-      <c r="D2427" t="inlineStr"/>
+      <c r="B2427" t="inlineStr">
+        <is>
+          <t>Arunesh RL</t>
+        </is>
+      </c>
+      <c r="C2427" t="inlineStr">
+        <is>
+          <t>arunesh2010092@ssn.edu.in</t>
+        </is>
+      </c>
+      <c r="D2427" t="inlineStr">
+        <is>
+          <t>Somalia</t>
+        </is>
+      </c>
       <c r="E2427" t="inlineStr">
         <is>
           <t>140813</t>
@@ -36844,9 +38380,21 @@
           <t>HR030</t>
         </is>
       </c>
-      <c r="B2428" t="inlineStr"/>
-      <c r="C2428" t="inlineStr"/>
-      <c r="D2428" t="inlineStr"/>
+      <c r="B2428" t="inlineStr">
+        <is>
+          <t>Shruthi.N</t>
+        </is>
+      </c>
+      <c r="C2428" t="inlineStr">
+        <is>
+          <t>shruthinagappan@gmail.com</t>
+        </is>
+      </c>
+      <c r="D2428" t="inlineStr">
+        <is>
+          <t>Ukraine</t>
+        </is>
+      </c>
       <c r="E2428" t="inlineStr">
         <is>
           <t>188555</t>
@@ -36859,9 +38407,21 @@
           <t>HR031</t>
         </is>
       </c>
-      <c r="B2429" t="inlineStr"/>
-      <c r="C2429" t="inlineStr"/>
-      <c r="D2429" t="inlineStr"/>
+      <c r="B2429" t="inlineStr">
+        <is>
+          <t>Lekha</t>
+        </is>
+      </c>
+      <c r="C2429" t="inlineStr">
+        <is>
+          <t>lekha2010182@ssn.edu.in</t>
+        </is>
+      </c>
+      <c r="D2429" t="inlineStr">
+        <is>
+          <t>Uruguay</t>
+        </is>
+      </c>
       <c r="E2429" t="inlineStr">
         <is>
           <t>270546</t>
@@ -36889,9 +38449,21 @@
           <t>HR033</t>
         </is>
       </c>
-      <c r="B2431" t="inlineStr"/>
-      <c r="C2431" t="inlineStr"/>
-      <c r="D2431" t="inlineStr"/>
+      <c r="B2431" t="inlineStr">
+        <is>
+          <t>Swathi G</t>
+        </is>
+      </c>
+      <c r="C2431" t="inlineStr">
+        <is>
+          <t>swathi2010640@ssn.edu.in</t>
+        </is>
+      </c>
+      <c r="D2431" t="inlineStr">
+        <is>
+          <t>FINLAND</t>
+        </is>
+      </c>
       <c r="E2431" t="inlineStr">
         <is>
           <t>428296</t>
@@ -36904,9 +38476,21 @@
           <t>HR034</t>
         </is>
       </c>
-      <c r="B2432" t="inlineStr"/>
-      <c r="C2432" t="inlineStr"/>
-      <c r="D2432" t="inlineStr"/>
+      <c r="B2432" t="inlineStr">
+        <is>
+          <t>K Swetha</t>
+        </is>
+      </c>
+      <c r="C2432" t="inlineStr">
+        <is>
+          <t>Swetha2010473@ssn.edu.in</t>
+        </is>
+      </c>
+      <c r="D2432" t="inlineStr">
+        <is>
+          <t>Iceland</t>
+        </is>
+      </c>
       <c r="E2432" t="inlineStr">
         <is>
           <t>542845</t>
@@ -36919,9 +38503,21 @@
           <t>HR035</t>
         </is>
       </c>
-      <c r="B2433" t="inlineStr"/>
-      <c r="C2433" t="inlineStr"/>
-      <c r="D2433" t="inlineStr"/>
+      <c r="B2433" t="inlineStr">
+        <is>
+          <t>Athmaaram S</t>
+        </is>
+      </c>
+      <c r="C2433" t="inlineStr">
+        <is>
+          <t>athmaaram1507@gmail.com</t>
+        </is>
+      </c>
+      <c r="D2433" t="inlineStr">
+        <is>
+          <t>Russian Federation</t>
+        </is>
+      </c>
       <c r="E2433" t="inlineStr">
         <is>
           <t>271872</t>
@@ -36934,9 +38530,21 @@
           <t>HR036</t>
         </is>
       </c>
-      <c r="B2434" t="inlineStr"/>
-      <c r="C2434" t="inlineStr"/>
-      <c r="D2434" t="inlineStr"/>
+      <c r="B2434" t="inlineStr">
+        <is>
+          <t>Hema M</t>
+        </is>
+      </c>
+      <c r="C2434" t="inlineStr">
+        <is>
+          <t>hemamohanavel2001@gmail.com</t>
+        </is>
+      </c>
+      <c r="D2434" t="inlineStr">
+        <is>
+          <t>Iraq</t>
+        </is>
+      </c>
       <c r="E2434" t="inlineStr">
         <is>
           <t>081445</t>
@@ -36949,9 +38557,21 @@
           <t>HR037</t>
         </is>
       </c>
-      <c r="B2435" t="inlineStr"/>
-      <c r="C2435" t="inlineStr"/>
-      <c r="D2435" t="inlineStr"/>
+      <c r="B2435" t="inlineStr">
+        <is>
+          <t>Asmita Sood</t>
+        </is>
+      </c>
+      <c r="C2435" t="inlineStr">
+        <is>
+          <t>as9743@srmist.edu.in</t>
+        </is>
+      </c>
+      <c r="D2435" t="inlineStr">
+        <is>
+          <t>Kenya</t>
+        </is>
+      </c>
       <c r="E2435" t="inlineStr">
         <is>
           <t>851293</t>
@@ -36979,9 +38599,21 @@
           <t>HR039</t>
         </is>
       </c>
-      <c r="B2437" t="inlineStr"/>
-      <c r="C2437" t="inlineStr"/>
-      <c r="D2437" t="inlineStr"/>
+      <c r="B2437" t="inlineStr">
+        <is>
+          <t>Raghul Pranavesh</t>
+        </is>
+      </c>
+      <c r="C2437" t="inlineStr">
+        <is>
+          <t>raghulpranavesh@gmail.com</t>
+        </is>
+      </c>
+      <c r="D2437" t="inlineStr">
+        <is>
+          <t>Saudi Arabia</t>
+        </is>
+      </c>
       <c r="E2437" t="inlineStr">
         <is>
           <t>188755</t>
@@ -36994,9 +38626,21 @@
           <t>HR040</t>
         </is>
       </c>
-      <c r="B2438" t="inlineStr"/>
-      <c r="C2438" t="inlineStr"/>
-      <c r="D2438" t="inlineStr"/>
+      <c r="B2438" t="inlineStr">
+        <is>
+          <t>Tejaswi s</t>
+        </is>
+      </c>
+      <c r="C2438" t="inlineStr">
+        <is>
+          <t>Tejaswis0702@gmail.com</t>
+        </is>
+      </c>
+      <c r="D2438" t="inlineStr">
+        <is>
+          <t>Spain</t>
+        </is>
+      </c>
       <c r="E2438" t="inlineStr">
         <is>
           <t>300437</t>
@@ -37909,9 +39553,21 @@
           <t>HR101</t>
         </is>
       </c>
-      <c r="B2499" t="inlineStr"/>
-      <c r="C2499" t="inlineStr"/>
-      <c r="D2499" t="inlineStr"/>
+      <c r="B2499" t="inlineStr">
+        <is>
+          <t>Ria Joseph</t>
+        </is>
+      </c>
+      <c r="C2499" t="inlineStr">
+        <is>
+          <t>riajoseph2002@gmail.com</t>
+        </is>
+      </c>
+      <c r="D2499" t="inlineStr">
+        <is>
+          <t>Armenia</t>
+        </is>
+      </c>
       <c r="E2499" t="inlineStr">
         <is>
           <t>845695</t>
@@ -37954,9 +39610,21 @@
           <t>HR104</t>
         </is>
       </c>
-      <c r="B2502" t="inlineStr"/>
-      <c r="C2502" t="inlineStr"/>
-      <c r="D2502" t="inlineStr"/>
+      <c r="B2502" t="inlineStr">
+        <is>
+          <t>Kanagambujam Venkatramani</t>
+        </is>
+      </c>
+      <c r="C2502" t="inlineStr">
+        <is>
+          <t>swekags02@gmail.com</t>
+        </is>
+      </c>
+      <c r="D2502" t="inlineStr">
+        <is>
+          <t>Brazil</t>
+        </is>
+      </c>
       <c r="E2502" t="inlineStr">
         <is>
           <t>751308</t>
@@ -38029,9 +39697,21 @@
           <t>HR109</t>
         </is>
       </c>
-      <c r="B2507" t="inlineStr"/>
-      <c r="C2507" t="inlineStr"/>
-      <c r="D2507" t="inlineStr"/>
+      <c r="B2507" t="inlineStr">
+        <is>
+          <t>Manasija Das</t>
+        </is>
+      </c>
+      <c r="C2507" t="inlineStr">
+        <is>
+          <t>dmanasija@gmail.com</t>
+        </is>
+      </c>
+      <c r="D2507" t="inlineStr">
+        <is>
+          <t>Denmark</t>
+        </is>
+      </c>
       <c r="E2507" t="inlineStr">
         <is>
           <t>063798</t>
@@ -38059,9 +39739,21 @@
           <t>HR111</t>
         </is>
       </c>
-      <c r="B2509" t="inlineStr"/>
-      <c r="C2509" t="inlineStr"/>
-      <c r="D2509" t="inlineStr"/>
+      <c r="B2509" t="inlineStr">
+        <is>
+          <t>Aruna Venkatesa Selvan</t>
+        </is>
+      </c>
+      <c r="C2509" t="inlineStr">
+        <is>
+          <t>19VCM09@wcc.edu.in</t>
+        </is>
+      </c>
+      <c r="D2509" t="inlineStr">
+        <is>
+          <t>Germany</t>
+        </is>
+      </c>
       <c r="E2509" t="inlineStr">
         <is>
           <t>469900</t>
@@ -38104,9 +39796,21 @@
           <t>HR114</t>
         </is>
       </c>
-      <c r="B2512" t="inlineStr"/>
-      <c r="C2512" t="inlineStr"/>
-      <c r="D2512" t="inlineStr"/>
+      <c r="B2512" t="inlineStr">
+        <is>
+          <t>Aarifa Khan</t>
+        </is>
+      </c>
+      <c r="C2512" t="inlineStr">
+        <is>
+          <t>aarifaku10@gmail.com</t>
+        </is>
+      </c>
+      <c r="D2512" t="inlineStr">
+        <is>
+          <t>Mauritania</t>
+        </is>
+      </c>
       <c r="E2512" t="inlineStr">
         <is>
           <t>067955</t>
@@ -38134,9 +39838,21 @@
           <t>HR116</t>
         </is>
       </c>
-      <c r="B2514" t="inlineStr"/>
-      <c r="C2514" t="inlineStr"/>
-      <c r="D2514" t="inlineStr"/>
+      <c r="B2514" t="inlineStr">
+        <is>
+          <t>Sibi Ranganathan</t>
+        </is>
+      </c>
+      <c r="C2514" t="inlineStr">
+        <is>
+          <t>sibiuthay3@gmail.com</t>
+        </is>
+      </c>
+      <c r="D2514" t="inlineStr">
+        <is>
+          <t>Nepal</t>
+        </is>
+      </c>
       <c r="E2514" t="inlineStr">
         <is>
           <t>136441</t>
@@ -38164,9 +39880,21 @@
           <t>HR118</t>
         </is>
       </c>
-      <c r="B2516" t="inlineStr"/>
-      <c r="C2516" t="inlineStr"/>
-      <c r="D2516" t="inlineStr"/>
+      <c r="B2516" t="inlineStr">
+        <is>
+          <t>Saranya Ravi</t>
+        </is>
+      </c>
+      <c r="C2516" t="inlineStr">
+        <is>
+          <t>saranyaravi2001@gmail.com</t>
+        </is>
+      </c>
+      <c r="D2516" t="inlineStr">
+        <is>
+          <t>Poland</t>
+        </is>
+      </c>
       <c r="E2516" t="inlineStr">
         <is>
           <t>181142</t>
@@ -38194,9 +39922,21 @@
           <t>HR120</t>
         </is>
       </c>
-      <c r="B2518" t="inlineStr"/>
-      <c r="C2518" t="inlineStr"/>
-      <c r="D2518" t="inlineStr"/>
+      <c r="B2518" t="inlineStr">
+        <is>
+          <t>Kathan Bhavsar</t>
+        </is>
+      </c>
+      <c r="C2518" t="inlineStr">
+        <is>
+          <t>kathanbhavsar25@gmail.com</t>
+        </is>
+      </c>
+      <c r="D2518" t="inlineStr">
+        <is>
+          <t>United Kingdom of Great Britain and Northern Ireland</t>
+        </is>
+      </c>
       <c r="E2518" t="inlineStr">
         <is>
           <t>633245</t>
@@ -38209,9 +39949,21 @@
           <t>HR121</t>
         </is>
       </c>
-      <c r="B2519" t="inlineStr"/>
-      <c r="C2519" t="inlineStr"/>
-      <c r="D2519" t="inlineStr"/>
+      <c r="B2519" t="inlineStr">
+        <is>
+          <t>Aruna Rajeswari KK</t>
+        </is>
+      </c>
+      <c r="C2519" t="inlineStr">
+        <is>
+          <t>aruna2001@mail.com</t>
+        </is>
+      </c>
+      <c r="D2519" t="inlineStr">
+        <is>
+          <t>Uzbekistan</t>
+        </is>
+      </c>
       <c r="E2519" t="inlineStr">
         <is>
           <t>998268</t>
@@ -38224,9 +39976,21 @@
           <t>HR122</t>
         </is>
       </c>
-      <c r="B2520" t="inlineStr"/>
-      <c r="C2520" t="inlineStr"/>
-      <c r="D2520" t="inlineStr"/>
+      <c r="B2520" t="inlineStr">
+        <is>
+          <t>Aishwarya S</t>
+        </is>
+      </c>
+      <c r="C2520" t="inlineStr">
+        <is>
+          <t>puppu2001@gmail.com</t>
+        </is>
+      </c>
+      <c r="D2520" t="inlineStr">
+        <is>
+          <t>Venezuela (Bolivarian Republic of)</t>
+        </is>
+      </c>
       <c r="E2520" t="inlineStr">
         <is>
           <t>157192</t>
@@ -38239,9 +40003,21 @@
           <t>HR123</t>
         </is>
       </c>
-      <c r="B2521" t="inlineStr"/>
-      <c r="C2521" t="inlineStr"/>
-      <c r="D2521" t="inlineStr"/>
+      <c r="B2521" t="inlineStr">
+        <is>
+          <t>Khushi Singh</t>
+        </is>
+      </c>
+      <c r="C2521" t="inlineStr">
+        <is>
+          <t>Khushi.singh2019@vitstudent.ac.in</t>
+        </is>
+      </c>
+      <c r="D2521" t="inlineStr">
+        <is>
+          <t>Canada</t>
+        </is>
+      </c>
       <c r="E2521" t="inlineStr">
         <is>
           <t>015046</t>
@@ -38254,9 +40030,21 @@
           <t>HR124</t>
         </is>
       </c>
-      <c r="B2522" t="inlineStr"/>
-      <c r="C2522" t="inlineStr"/>
-      <c r="D2522" t="inlineStr"/>
+      <c r="B2522" t="inlineStr">
+        <is>
+          <t>Gayathri Arvind</t>
+        </is>
+      </c>
+      <c r="C2522" t="inlineStr">
+        <is>
+          <t>gayathriarvind0404@gmail.com</t>
+        </is>
+      </c>
+      <c r="D2522" t="inlineStr">
+        <is>
+          <t>South Africa</t>
+        </is>
+      </c>
       <c r="E2522" t="inlineStr">
         <is>
           <t>999075</t>
@@ -38269,9 +40057,21 @@
           <t>HR125</t>
         </is>
       </c>
-      <c r="B2523" t="inlineStr"/>
-      <c r="C2523" t="inlineStr"/>
-      <c r="D2523" t="inlineStr"/>
+      <c r="B2523" t="inlineStr">
+        <is>
+          <t>Sneha Nair</t>
+        </is>
+      </c>
+      <c r="C2523" t="inlineStr">
+        <is>
+          <t>snehan665@gmail.com</t>
+        </is>
+      </c>
+      <c r="D2523" t="inlineStr">
+        <is>
+          <t>Sri Lanka</t>
+        </is>
+      </c>
       <c r="E2523" t="inlineStr">
         <is>
           <t>094982</t>
@@ -38284,9 +40084,21 @@
           <t>HR126</t>
         </is>
       </c>
-      <c r="B2524" t="inlineStr"/>
-      <c r="C2524" t="inlineStr"/>
-      <c r="D2524" t="inlineStr"/>
+      <c r="B2524" t="inlineStr">
+        <is>
+          <t>Kiran Srinivasan</t>
+        </is>
+      </c>
+      <c r="C2524" t="inlineStr">
+        <is>
+          <t>kiransrini9@gmail.com</t>
+        </is>
+      </c>
+      <c r="D2524" t="inlineStr">
+        <is>
+          <t>Switzerland</t>
+        </is>
+      </c>
       <c r="E2524" t="inlineStr">
         <is>
           <t>034691</t>
@@ -39409,9 +41221,21 @@
           <t>HR201</t>
         </is>
       </c>
-      <c r="B2599" t="inlineStr"/>
-      <c r="C2599" t="inlineStr"/>
-      <c r="D2599" t="inlineStr"/>
+      <c r="B2599" t="inlineStr">
+        <is>
+          <t>Tinashree</t>
+        </is>
+      </c>
+      <c r="C2599" t="inlineStr">
+        <is>
+          <t>tinashree.chowdary@law.christuniversity.in</t>
+        </is>
+      </c>
+      <c r="D2599" t="inlineStr">
+        <is>
+          <t>Austria</t>
+        </is>
+      </c>
       <c r="E2599" t="inlineStr">
         <is>
           <t>703494</t>
@@ -39424,9 +41248,21 @@
           <t>HR202</t>
         </is>
       </c>
-      <c r="B2600" t="inlineStr"/>
-      <c r="C2600" t="inlineStr"/>
-      <c r="D2600" t="inlineStr"/>
+      <c r="B2600" t="inlineStr">
+        <is>
+          <t>Apurba Ranjan</t>
+        </is>
+      </c>
+      <c r="C2600" t="inlineStr">
+        <is>
+          <t>apurba.ranjan2020@vitstudent.ac.in</t>
+        </is>
+      </c>
+      <c r="D2600" t="inlineStr">
+        <is>
+          <t>Bangladesh</t>
+        </is>
+      </c>
       <c r="E2600" t="inlineStr">
         <is>
           <t>093887</t>
@@ -39439,9 +41275,21 @@
           <t>HR203</t>
         </is>
       </c>
-      <c r="B2601" t="inlineStr"/>
-      <c r="C2601" t="inlineStr"/>
-      <c r="D2601" t="inlineStr"/>
+      <c r="B2601" t="inlineStr">
+        <is>
+          <t>Sherlline Josephin</t>
+        </is>
+      </c>
+      <c r="C2601" t="inlineStr">
+        <is>
+          <t>sherllinejose@gmail.com</t>
+        </is>
+      </c>
+      <c r="D2601" t="inlineStr">
+        <is>
+          <t>Burkina Faso</t>
+        </is>
+      </c>
       <c r="E2601" t="inlineStr">
         <is>
           <t>309970</t>
@@ -39469,9 +41317,21 @@
           <t>HR205</t>
         </is>
       </c>
-      <c r="B2603" t="inlineStr"/>
-      <c r="C2603" t="inlineStr"/>
-      <c r="D2603" t="inlineStr"/>
+      <c r="B2603" t="inlineStr">
+        <is>
+          <t>Chandrasekhar Ananthabhotla</t>
+        </is>
+      </c>
+      <c r="C2603" t="inlineStr">
+        <is>
+          <t>chandrasekhar.acss@gmail.com</t>
+        </is>
+      </c>
+      <c r="D2603" t="inlineStr">
+        <is>
+          <t>Côte d’Ivoire</t>
+        </is>
+      </c>
       <c r="E2603" t="inlineStr">
         <is>
           <t>065827</t>
@@ -39484,9 +41344,21 @@
           <t>HR206</t>
         </is>
       </c>
-      <c r="B2604" t="inlineStr"/>
-      <c r="C2604" t="inlineStr"/>
-      <c r="D2604" t="inlineStr"/>
+      <c r="B2604" t="inlineStr">
+        <is>
+          <t>Aditi Goel</t>
+        </is>
+      </c>
+      <c r="C2604" t="inlineStr">
+        <is>
+          <t>goela9195@gmail.com</t>
+        </is>
+      </c>
+      <c r="D2604" t="inlineStr">
+        <is>
+          <t>Czechia</t>
+        </is>
+      </c>
       <c r="E2604" t="inlineStr">
         <is>
           <t>023412</t>
@@ -39499,9 +41371,21 @@
           <t>HR207</t>
         </is>
       </c>
-      <c r="B2605" t="inlineStr"/>
-      <c r="C2605" t="inlineStr"/>
-      <c r="D2605" t="inlineStr"/>
+      <c r="B2605" t="inlineStr">
+        <is>
+          <t>Sri Moukthika</t>
+        </is>
+      </c>
+      <c r="C2605" t="inlineStr">
+        <is>
+          <t>20jgls-smvadlapatla@jgu.edu.in</t>
+        </is>
+      </c>
+      <c r="D2605" t="inlineStr">
+        <is>
+          <t>Gabon</t>
+        </is>
+      </c>
       <c r="E2605" t="inlineStr">
         <is>
           <t>261312</t>
@@ -39514,9 +41398,21 @@
           <t>HR208</t>
         </is>
       </c>
-      <c r="B2606" t="inlineStr"/>
-      <c r="C2606" t="inlineStr"/>
-      <c r="D2606" t="inlineStr"/>
+      <c r="B2606" t="inlineStr">
+        <is>
+          <t>Abhilash Madabhushi</t>
+        </is>
+      </c>
+      <c r="C2606" t="inlineStr">
+        <is>
+          <t>abhilashr490@gmail.com</t>
+        </is>
+      </c>
+      <c r="D2606" t="inlineStr">
+        <is>
+          <t>India</t>
+        </is>
+      </c>
       <c r="E2606" t="inlineStr">
         <is>
           <t>665336</t>
@@ -39574,9 +41470,21 @@
           <t>HR212</t>
         </is>
       </c>
-      <c r="B2610" t="inlineStr"/>
-      <c r="C2610" t="inlineStr"/>
-      <c r="D2610" t="inlineStr"/>
+      <c r="B2610" t="inlineStr">
+        <is>
+          <t>Harish Kumar</t>
+        </is>
+      </c>
+      <c r="C2610" t="inlineStr">
+        <is>
+          <t>harishkumar1452001@gmail.com</t>
+        </is>
+      </c>
+      <c r="D2610" t="inlineStr">
+        <is>
+          <t>Netherlands</t>
+        </is>
+      </c>
       <c r="E2610" t="inlineStr">
         <is>
           <t>832640</t>
@@ -39619,9 +41527,21 @@
           <t>HR215</t>
         </is>
       </c>
-      <c r="B2613" t="inlineStr"/>
-      <c r="C2613" t="inlineStr"/>
-      <c r="D2613" t="inlineStr"/>
+      <c r="B2613" t="inlineStr">
+        <is>
+          <t>Roshan Raju</t>
+        </is>
+      </c>
+      <c r="C2613" t="inlineStr">
+        <is>
+          <t>roshan.raju@law.christuniversity.in</t>
+        </is>
+      </c>
+      <c r="D2613" t="inlineStr">
+        <is>
+          <t>Togo</t>
+        </is>
+      </c>
       <c r="E2613" t="inlineStr">
         <is>
           <t>395250</t>
@@ -39649,9 +41569,21 @@
           <t>HR217</t>
         </is>
       </c>
-      <c r="B2615" t="inlineStr"/>
-      <c r="C2615" t="inlineStr"/>
-      <c r="D2615" t="inlineStr"/>
+      <c r="B2615" t="inlineStr">
+        <is>
+          <t>Darsh Kumar</t>
+        </is>
+      </c>
+      <c r="C2615" t="inlineStr">
+        <is>
+          <t>darsh.kumar2002@gmail.com</t>
+        </is>
+      </c>
+      <c r="D2615" t="inlineStr">
+        <is>
+          <t>Rwanda</t>
+        </is>
+      </c>
       <c r="E2615" t="inlineStr">
         <is>
           <t>369917</t>
@@ -39664,9 +41596,21 @@
           <t>HR218</t>
         </is>
       </c>
-      <c r="B2616" t="inlineStr"/>
-      <c r="C2616" t="inlineStr"/>
-      <c r="D2616" t="inlineStr"/>
+      <c r="B2616" t="inlineStr">
+        <is>
+          <t>Anupama Nhavalore</t>
+        </is>
+      </c>
+      <c r="C2616" t="inlineStr">
+        <is>
+          <t>anupama.n.nair16@gmail.com</t>
+        </is>
+      </c>
+      <c r="D2616" t="inlineStr">
+        <is>
+          <t>United Arab Emirates</t>
+        </is>
+      </c>
       <c r="E2616" t="inlineStr">
         <is>
           <t>213374</t>
@@ -39679,9 +41623,21 @@
           <t>HR219</t>
         </is>
       </c>
-      <c r="B2617" t="inlineStr"/>
-      <c r="C2617" t="inlineStr"/>
-      <c r="D2617" t="inlineStr"/>
+      <c r="B2617" t="inlineStr">
+        <is>
+          <t>Jhethru V</t>
+        </is>
+      </c>
+      <c r="C2617" t="inlineStr">
+        <is>
+          <t>jhethru.v@law.christuniversity.in</t>
+        </is>
+      </c>
+      <c r="D2617" t="inlineStr">
+        <is>
+          <t>United States of America</t>
+        </is>
+      </c>
       <c r="E2617" t="inlineStr">
         <is>
           <t>924515</t>
@@ -39694,9 +41650,21 @@
           <t>HR220</t>
         </is>
       </c>
-      <c r="B2618" t="inlineStr"/>
-      <c r="C2618" t="inlineStr"/>
-      <c r="D2618" t="inlineStr"/>
+      <c r="B2618" t="inlineStr">
+        <is>
+          <t>Anuj Jacob</t>
+        </is>
+      </c>
+      <c r="C2618" t="inlineStr">
+        <is>
+          <t>anuj_j.sias19@krea.ac.in</t>
+        </is>
+      </c>
+      <c r="D2618" t="inlineStr">
+        <is>
+          <t>Egypt</t>
+        </is>
+      </c>
       <c r="E2618" t="inlineStr">
         <is>
           <t>465961</t>
@@ -42394,9 +44362,21 @@
           <t>HR400</t>
         </is>
       </c>
-      <c r="B2798" t="inlineStr"/>
-      <c r="C2798" t="inlineStr"/>
-      <c r="D2798" t="inlineStr"/>
+      <c r="B2798" t="inlineStr">
+        <is>
+          <t>Saiansh Raizada</t>
+        </is>
+      </c>
+      <c r="C2798" t="inlineStr">
+        <is>
+          <t>saiansh.raizada@gmail.com</t>
+        </is>
+      </c>
+      <c r="D2798" t="inlineStr">
+        <is>
+          <t>Iran</t>
+        </is>
+      </c>
       <c r="E2798" t="inlineStr">
         <is>
           <t>755452</t>
@@ -46999,9 +48979,21 @@
           <t>HR707</t>
         </is>
       </c>
-      <c r="B3105" t="inlineStr"/>
-      <c r="C3105" t="inlineStr"/>
-      <c r="D3105" t="inlineStr"/>
+      <c r="B3105" t="inlineStr">
+        <is>
+          <t>Mahalakshmi</t>
+        </is>
+      </c>
+      <c r="C3105" t="inlineStr">
+        <is>
+          <t>mahalakshmi_1307@yahoo.co.in</t>
+        </is>
+      </c>
+      <c r="D3105" t="inlineStr">
+        <is>
+          <t>International Press 1</t>
+        </is>
+      </c>
       <c r="E3105" t="inlineStr">
         <is>
           <t>658566</t>
@@ -47014,9 +49006,21 @@
           <t>HR708</t>
         </is>
       </c>
-      <c r="B3106" t="inlineStr"/>
-      <c r="C3106" t="inlineStr"/>
-      <c r="D3106" t="inlineStr"/>
+      <c r="B3106" t="inlineStr">
+        <is>
+          <t>Amrita Sathyananthan</t>
+        </is>
+      </c>
+      <c r="C3106" t="inlineStr">
+        <is>
+          <t>amritsathyananthan@gmail.com</t>
+        </is>
+      </c>
+      <c r="D3106" t="inlineStr">
+        <is>
+          <t>International Press 2</t>
+        </is>
+      </c>
       <c r="E3106" t="inlineStr">
         <is>
           <t>430584</t>
@@ -47044,9 +49048,21 @@
           <t>HR710</t>
         </is>
       </c>
-      <c r="B3108" t="inlineStr"/>
-      <c r="C3108" t="inlineStr"/>
-      <c r="D3108" t="inlineStr"/>
+      <c r="B3108" t="inlineStr">
+        <is>
+          <t>Siddharth Lavu</t>
+        </is>
+      </c>
+      <c r="C3108" t="inlineStr">
+        <is>
+          <t>lavusiddharth@gmail.com</t>
+        </is>
+      </c>
+      <c r="D3108" t="inlineStr">
+        <is>
+          <t>International Press 3</t>
+        </is>
+      </c>
       <c r="E3108" t="inlineStr">
         <is>
           <t>589104</t>

</xml_diff>